<commit_message>
ScriptedPlayback is still unknown in function, but Dash is the one which makes the buffering pause when the video is paused.
</commit_message>
<xml_diff>
--- a/Translation.xlsx
+++ b/Translation.xlsx
@@ -309,10 +309,10 @@
     <t>Detecció automàtica</t>
   </si>
   <si>
-    <t>SETTINGS_SCRIPTEDPLAYBACK</t>
-  </si>
-  <si>
-    <t>Scripted Playback</t>
+    <t>SETTINGS_DASHPLAYBACK</t>
+  </si>
+  <si>
+    <t>Dash Playback</t>
   </si>
   <si>
     <t>SETTINGS_FLEXWIDTHONPAGE_LABEL</t>
@@ -11232,10 +11232,10 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="49" borderId="0" fontId="0" applyNumberFormat="1">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="49" borderId="0" applyFont="1" fontId="1" applyNumberFormat="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="49" borderId="0" applyFont="1" fontId="1" applyNumberFormat="1">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="49" borderId="0" fontId="0" applyNumberFormat="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="49" borderId="0" fontId="0" applyNumberFormat="1">
@@ -11291,82 +11291,82 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c s="2" r="A1"/>
-      <c t="s" s="2" r="B1">
+      <c s="1" r="A1"/>
+      <c t="s" s="1" r="B1">
         <v>0</v>
       </c>
-      <c t="s" s="2" r="C1">
+      <c t="s" s="1" r="C1">
         <v>1</v>
       </c>
-      <c t="s" s="2" r="D1">
+      <c t="s" s="1" r="D1">
         <v>2</v>
       </c>
-      <c t="s" s="2" r="E1">
+      <c t="s" s="1" r="E1">
         <v>3</v>
       </c>
-      <c t="s" s="2" r="F1">
+      <c t="s" s="1" r="F1">
         <v>4</v>
       </c>
-      <c t="s" s="2" r="G1">
+      <c t="s" s="1" r="G1">
         <v>5</v>
       </c>
-      <c t="s" s="2" r="H1">
+      <c t="s" s="1" r="H1">
         <v>6</v>
       </c>
-      <c t="s" s="2" r="I1">
+      <c t="s" s="1" r="I1">
         <v>7</v>
       </c>
-      <c t="s" s="2" r="J1">
+      <c t="s" s="1" r="J1">
         <v>8</v>
       </c>
-      <c t="s" s="2" r="K1">
+      <c t="s" s="1" r="K1">
         <v>9</v>
       </c>
-      <c t="s" s="2" r="L1">
+      <c t="s" s="1" r="L1">
         <v>10</v>
       </c>
-      <c t="s" s="2" r="M1">
+      <c t="s" s="1" r="M1">
         <v>11</v>
       </c>
-      <c t="s" s="2" r="N1">
+      <c t="s" s="1" r="N1">
         <v>12</v>
       </c>
-      <c t="s" s="2" r="O1">
+      <c t="s" s="1" r="O1">
         <v>13</v>
       </c>
-      <c t="s" s="2" r="P1">
+      <c t="s" s="1" r="P1">
         <v>14</v>
       </c>
-      <c t="s" s="2" r="Q1">
+      <c t="s" s="1" r="Q1">
         <v>15</v>
       </c>
-      <c t="s" s="2" r="R1">
+      <c t="s" s="1" r="R1">
         <v>16</v>
       </c>
-      <c t="s" s="2" r="S1">
+      <c t="s" s="1" r="S1">
         <v>17</v>
       </c>
-      <c t="s" s="2" r="T1">
+      <c t="s" s="1" r="T1">
         <v>18</v>
       </c>
-      <c t="s" s="2" r="U1">
+      <c t="s" s="1" r="U1">
         <v>19</v>
       </c>
-      <c t="s" s="2" r="V1">
+      <c t="s" s="1" r="V1">
         <v>20</v>
       </c>
-      <c t="s" s="2" r="W1">
+      <c t="s" s="1" r="W1">
         <v>21</v>
       </c>
-      <c t="s" s="2" r="X1">
+      <c t="s" s="1" r="X1">
         <v>22</v>
       </c>
-      <c t="s" s="2" r="Y1">
+      <c t="s" s="1" r="Y1">
         <v>23</v>
       </c>
     </row>
     <row r="2">
-      <c t="s" s="2" r="A2">
+      <c t="s" s="1" r="A2">
         <v>24</v>
       </c>
       <c t="s" s="3" r="B2">
@@ -11443,7 +11443,7 @@
       </c>
     </row>
     <row r="3">
-      <c t="s" s="2" r="A3">
+      <c t="s" s="1" r="A3">
         <v>49</v>
       </c>
       <c t="s" s="3" r="B3">
@@ -11520,7 +11520,7 @@
       </c>
     </row>
     <row r="4">
-      <c t="s" s="2" r="A4">
+      <c t="s" s="1" r="A4">
         <v>73</v>
       </c>
       <c t="s" s="3" r="B4">
@@ -11597,7 +11597,7 @@
       </c>
     </row>
     <row r="5">
-      <c t="s" s="2" r="A5">
+      <c t="s" s="1" r="A5">
         <v>98</v>
       </c>
       <c t="s" s="3" r="B5">
@@ -11628,7 +11628,7 @@
       <c s="3" r="Y5"/>
     </row>
     <row r="6">
-      <c t="s" s="2" r="A6">
+      <c t="s" s="1" r="A6">
         <v>100</v>
       </c>
       <c t="s" s="3" r="B6">
@@ -11671,7 +11671,7 @@
       <c s="3" r="Y6"/>
     </row>
     <row r="7">
-      <c t="s" s="2" r="A7">
+      <c t="s" s="1" r="A7">
         <v>108</v>
       </c>
       <c t="s" s="3" r="B7">
@@ -11718,7 +11718,7 @@
       </c>
     </row>
     <row r="8">
-      <c t="s" s="2" r="A8">
+      <c t="s" s="1" r="A8">
         <v>118</v>
       </c>
       <c t="s" s="3" r="B8">
@@ -11763,7 +11763,7 @@
       </c>
     </row>
     <row r="9">
-      <c t="s" s="2" r="A9">
+      <c t="s" s="1" r="A9">
         <v>127</v>
       </c>
       <c t="s" s="3" r="B9">
@@ -11808,7 +11808,7 @@
       </c>
     </row>
     <row r="10">
-      <c t="s" s="2" r="A10">
+      <c t="s" s="1" r="A10">
         <v>135</v>
       </c>
       <c t="s" s="3" r="B10">
@@ -11853,7 +11853,7 @@
       </c>
     </row>
     <row r="11">
-      <c t="s" s="2" r="A11">
+      <c t="s" s="1" r="A11">
         <v>144</v>
       </c>
       <c t="s" s="3" r="B11">
@@ -11898,7 +11898,7 @@
       </c>
     </row>
     <row r="12">
-      <c t="s" s="2" r="A12">
+      <c t="s" s="1" r="A12">
         <v>153</v>
       </c>
       <c t="s" s="3" r="B12">
@@ -11943,7 +11943,7 @@
       </c>
     </row>
     <row r="13">
-      <c t="s" s="2" r="A13">
+      <c t="s" s="1" r="A13">
         <v>162</v>
       </c>
       <c t="s" s="3" r="B13">
@@ -11988,7 +11988,7 @@
       </c>
     </row>
     <row r="14">
-      <c t="s" s="2" r="A14">
+      <c t="s" s="1" r="A14">
         <v>171</v>
       </c>
       <c t="s" s="3" r="B14">
@@ -12033,7 +12033,7 @@
       </c>
     </row>
     <row r="15">
-      <c t="s" s="2" r="A15">
+      <c t="s" s="1" r="A15">
         <v>179</v>
       </c>
       <c t="s" s="3" r="B15">
@@ -12078,7 +12078,7 @@
       </c>
     </row>
     <row r="16">
-      <c t="s" s="2" r="A16">
+      <c t="s" s="1" r="A16">
         <v>188</v>
       </c>
       <c t="s" s="3" r="B16">
@@ -12123,7 +12123,7 @@
       </c>
     </row>
     <row r="17">
-      <c t="s" s="2" r="A17">
+      <c t="s" s="1" r="A17">
         <v>197</v>
       </c>
       <c t="s" s="3" r="B17">
@@ -12168,7 +12168,7 @@
       </c>
     </row>
     <row r="18">
-      <c t="s" s="2" r="A18">
+      <c t="s" s="1" r="A18">
         <v>206</v>
       </c>
       <c t="s" s="3" r="B18">
@@ -12213,7 +12213,7 @@
       </c>
     </row>
     <row r="19">
-      <c t="s" s="2" r="A19">
+      <c t="s" s="1" r="A19">
         <v>214</v>
       </c>
       <c t="s" s="3" r="B19">
@@ -12268,7 +12268,7 @@
       </c>
     </row>
     <row r="20">
-      <c t="s" s="2" r="A20">
+      <c t="s" s="1" r="A20">
         <v>228</v>
       </c>
       <c t="s" s="3" r="B20">
@@ -12323,7 +12323,7 @@
       </c>
     </row>
     <row r="21">
-      <c t="s" s="2" r="A21">
+      <c t="s" s="1" r="A21">
         <v>242</v>
       </c>
       <c t="s" s="3" r="B21">
@@ -12378,7 +12378,7 @@
       </c>
     </row>
     <row r="22">
-      <c t="s" s="2" r="A22">
+      <c t="s" s="1" r="A22">
         <v>254</v>
       </c>
       <c t="s" s="3" r="B22">
@@ -12437,7 +12437,7 @@
       </c>
     </row>
     <row r="23">
-      <c t="s" s="2" r="A23">
+      <c t="s" s="1" r="A23">
         <v>269</v>
       </c>
       <c t="s" s="3" r="B23">
@@ -12498,7 +12498,7 @@
       </c>
     </row>
     <row r="24">
-      <c t="s" s="2" r="A24">
+      <c t="s" s="1" r="A24">
         <v>282</v>
       </c>
       <c t="s" s="3" r="B24">
@@ -12557,7 +12557,7 @@
       </c>
     </row>
     <row r="25">
-      <c t="s" s="2" r="A25">
+      <c t="s" s="1" r="A25">
         <v>284</v>
       </c>
       <c t="s" s="3" r="B25">
@@ -12618,7 +12618,7 @@
       </c>
     </row>
     <row r="26">
-      <c t="s" s="2" r="A26">
+      <c t="s" s="1" r="A26">
         <v>300</v>
       </c>
       <c t="s" s="3" r="B26">
@@ -12679,7 +12679,7 @@
       </c>
     </row>
     <row r="27">
-      <c t="s" s="2" r="A27">
+      <c t="s" s="1" r="A27">
         <v>316</v>
       </c>
       <c t="s" s="3" r="B27">
@@ -12740,7 +12740,7 @@
       </c>
     </row>
     <row r="28">
-      <c t="s" s="2" r="A28">
+      <c t="s" s="1" r="A28">
         <v>332</v>
       </c>
       <c t="s" s="3" r="B28">
@@ -12803,7 +12803,7 @@
       </c>
     </row>
     <row r="29">
-      <c t="s" s="2" r="A29">
+      <c t="s" s="1" r="A29">
         <v>347</v>
       </c>
       <c t="s" s="3" r="B29">
@@ -12868,7 +12868,7 @@
       </c>
     </row>
     <row r="30">
-      <c t="s" s="2" r="A30">
+      <c t="s" s="1" r="A30">
         <v>364</v>
       </c>
       <c t="s" s="3" r="B30">
@@ -12933,7 +12933,7 @@
       </c>
     </row>
     <row r="31">
-      <c t="s" s="2" r="A31">
+      <c t="s" s="1" r="A31">
         <v>381</v>
       </c>
       <c t="s" s="3" r="B31">
@@ -12996,7 +12996,7 @@
       </c>
     </row>
     <row r="32">
-      <c t="s" s="2" r="A32">
+      <c t="s" s="1" r="A32">
         <v>397</v>
       </c>
       <c t="s" s="3" r="B32">
@@ -13059,7 +13059,7 @@
       </c>
     </row>
     <row r="33">
-      <c t="s" s="2" r="A33">
+      <c t="s" s="1" r="A33">
         <v>412</v>
       </c>
       <c t="s" s="3" r="B33">
@@ -13122,7 +13122,7 @@
       </c>
     </row>
     <row r="34">
-      <c t="s" s="2" r="A34">
+      <c t="s" s="1" r="A34">
         <v>421</v>
       </c>
       <c t="s" s="3" r="B34">
@@ -13185,7 +13185,7 @@
       </c>
     </row>
     <row r="35">
-      <c t="s" s="2" r="A35">
+      <c t="s" s="1" r="A35">
         <v>430</v>
       </c>
       <c t="s" s="3" r="B35">
@@ -13248,7 +13248,7 @@
       </c>
     </row>
     <row r="36">
-      <c t="s" s="2" r="A36">
+      <c t="s" s="1" r="A36">
         <v>445</v>
       </c>
       <c t="s" s="3" r="B36">
@@ -13311,7 +13311,7 @@
       </c>
     </row>
     <row r="37">
-      <c t="s" s="2" r="A37">
+      <c t="s" s="1" r="A37">
         <v>459</v>
       </c>
       <c t="s" s="3" r="B37">
@@ -13374,7 +13374,7 @@
       </c>
     </row>
     <row r="38">
-      <c t="s" s="2" r="A38">
+      <c t="s" s="1" r="A38">
         <v>476</v>
       </c>
       <c t="s" s="3" r="B38">
@@ -13437,7 +13437,7 @@
       </c>
     </row>
     <row r="39">
-      <c t="s" s="2" r="A39">
+      <c t="s" s="1" r="A39">
         <v>493</v>
       </c>
       <c t="s" s="3" r="B39">
@@ -13498,7 +13498,7 @@
       </c>
     </row>
     <row r="40">
-      <c t="s" s="2" r="A40">
+      <c t="s" s="1" r="A40">
         <v>509</v>
       </c>
       <c t="s" s="3" r="B40">
@@ -13561,7 +13561,7 @@
       </c>
     </row>
     <row r="41">
-      <c t="s" s="2" r="A41">
+      <c t="s" s="1" r="A41">
         <v>512</v>
       </c>
       <c t="s" s="3" r="B41">
@@ -13622,7 +13622,7 @@
       </c>
     </row>
     <row r="42">
-      <c t="s" s="2" r="A42">
+      <c t="s" s="1" r="A42">
         <v>523</v>
       </c>
       <c t="s" s="3" r="B42">
@@ -13685,7 +13685,7 @@
       </c>
     </row>
     <row r="43">
-      <c t="s" s="2" r="A43">
+      <c t="s" s="1" r="A43">
         <v>536</v>
       </c>
       <c t="s" s="3" r="B43">
@@ -13746,7 +13746,7 @@
       </c>
     </row>
     <row r="44">
-      <c t="s" s="2" r="A44">
+      <c t="s" s="1" r="A44">
         <v>552</v>
       </c>
       <c t="s" s="3" r="B44">
@@ -13809,7 +13809,7 @@
       </c>
     </row>
     <row r="45">
-      <c t="s" s="2" r="A45">
+      <c t="s" s="1" r="A45">
         <v>569</v>
       </c>
       <c t="s" s="3" r="B45">
@@ -13872,7 +13872,7 @@
       </c>
     </row>
     <row r="46">
-      <c t="s" s="2" r="A46">
+      <c t="s" s="1" r="A46">
         <v>585</v>
       </c>
       <c t="s" s="3" r="B46">
@@ -13931,7 +13931,7 @@
       </c>
     </row>
     <row r="47">
-      <c t="s" s="2" r="A47">
+      <c t="s" s="1" r="A47">
         <v>589</v>
       </c>
       <c t="s" s="3" r="B47">
@@ -13994,7 +13994,7 @@
       </c>
     </row>
     <row r="48">
-      <c t="s" s="2" r="A48">
+      <c t="s" s="1" r="A48">
         <v>602</v>
       </c>
       <c t="s" s="3" r="B48">
@@ -14057,7 +14057,7 @@
       </c>
     </row>
     <row r="49">
-      <c t="s" s="2" r="A49">
+      <c t="s" s="1" r="A49">
         <v>614</v>
       </c>
       <c t="s" s="3" r="B49">
@@ -14122,7 +14122,7 @@
       </c>
     </row>
     <row r="50">
-      <c t="s" s="2" r="A50">
+      <c t="s" s="1" r="A50">
         <v>632</v>
       </c>
       <c t="s" s="3" r="B50">
@@ -14187,7 +14187,7 @@
       </c>
     </row>
     <row r="51">
-      <c t="s" s="2" r="A51">
+      <c t="s" s="1" r="A51">
         <v>650</v>
       </c>
       <c t="s" s="3" r="B51">
@@ -14252,7 +14252,7 @@
       </c>
     </row>
     <row r="52">
-      <c t="s" s="2" r="A52">
+      <c t="s" s="1" r="A52">
         <v>668</v>
       </c>
       <c t="s" s="3" r="B52">
@@ -14315,7 +14315,7 @@
       </c>
     </row>
     <row r="53">
-      <c t="s" s="2" r="A53">
+      <c t="s" s="1" r="A53">
         <v>686</v>
       </c>
       <c t="s" s="3" r="B53">
@@ -14376,38 +14376,38 @@
       </c>
     </row>
     <row r="54">
-      <c t="s" s="2" r="A54">
+      <c t="s" s="1" r="A54">
         <v>701</v>
       </c>
-      <c t="s" s="1" r="B54">
+      <c t="s" s="2" r="B54">
         <v>702</v>
       </c>
-      <c t="s" s="1" r="C54">
+      <c t="s" s="2" r="C54">
         <v>702</v>
       </c>
-      <c t="s" s="1" r="D54">
+      <c t="s" s="2" r="D54">
         <v>702</v>
       </c>
       <c s="3" r="E54"/>
       <c s="3" r="F54"/>
       <c s="3" r="G54"/>
       <c s="3" r="H54"/>
-      <c t="s" s="1" r="I54">
+      <c t="s" s="2" r="I54">
         <v>702</v>
       </c>
       <c t="s" s="3" r="J54">
         <v>703</v>
       </c>
       <c s="3" r="K54"/>
-      <c t="s" s="1" r="L54">
+      <c t="s" s="2" r="L54">
         <v>702</v>
       </c>
-      <c t="s" s="1" r="M54">
+      <c t="s" s="2" r="M54">
         <v>702</v>
       </c>
       <c s="3" r="N54"/>
       <c s="3" r="O54"/>
-      <c t="s" s="1" r="P54">
+      <c t="s" s="2" r="P54">
         <v>702</v>
       </c>
       <c t="s" s="3" r="Q54">
@@ -14419,7 +14419,7 @@
       <c t="s" s="3" r="S54">
         <v>702</v>
       </c>
-      <c t="s" s="1" r="T54">
+      <c t="s" s="2" r="T54">
         <v>702</v>
       </c>
       <c s="3" r="U54"/>
@@ -14432,12 +14432,12 @@
       <c t="s" s="3" r="X54">
         <v>702</v>
       </c>
-      <c t="s" s="1" r="Y54">
+      <c t="s" s="2" r="Y54">
         <v>702</v>
       </c>
     </row>
     <row r="55">
-      <c t="s" s="2" r="A55">
+      <c t="s" s="1" r="A55">
         <v>704</v>
       </c>
       <c t="s" s="3" r="B55">
@@ -14502,7 +14502,7 @@
       </c>
     </row>
     <row r="56">
-      <c t="s" s="2" r="A56">
+      <c t="s" s="1" r="A56">
         <v>710</v>
       </c>
       <c t="s" s="3" r="B56">
@@ -14567,7 +14567,7 @@
       </c>
     </row>
     <row r="57">
-      <c t="s" s="2" r="A57">
+      <c t="s" s="1" r="A57">
         <v>725</v>
       </c>
       <c t="s" s="3" r="B57">
@@ -14636,7 +14636,7 @@
       </c>
     </row>
     <row r="58">
-      <c t="s" s="2" r="A58">
+      <c t="s" s="1" r="A58">
         <v>745</v>
       </c>
       <c t="s" s="3" r="B58">
@@ -14705,7 +14705,7 @@
       </c>
     </row>
     <row r="59">
-      <c t="s" s="2" r="A59">
+      <c t="s" s="1" r="A59">
         <v>764</v>
       </c>
       <c t="s" s="3" r="B59">
@@ -14774,7 +14774,7 @@
       </c>
     </row>
     <row r="60">
-      <c t="s" s="2" r="A60">
+      <c t="s" s="1" r="A60">
         <v>783</v>
       </c>
       <c t="s" s="3" r="B60">
@@ -14843,7 +14843,7 @@
       </c>
     </row>
     <row r="61">
-      <c t="s" s="2" r="A61">
+      <c t="s" s="1" r="A61">
         <v>802</v>
       </c>
       <c t="s" s="3" r="B61">
@@ -14912,7 +14912,7 @@
       </c>
     </row>
     <row r="62">
-      <c t="s" s="2" r="A62">
+      <c t="s" s="1" r="A62">
         <v>821</v>
       </c>
       <c t="s" s="3" r="B62">
@@ -14981,7 +14981,7 @@
       </c>
     </row>
     <row r="63">
-      <c t="s" s="2" r="A63">
+      <c t="s" s="1" r="A63">
         <v>840</v>
       </c>
       <c t="s" s="3" r="B63">
@@ -15050,7 +15050,7 @@
       </c>
     </row>
     <row r="64">
-      <c t="s" s="2" r="A64">
+      <c t="s" s="1" r="A64">
         <v>860</v>
       </c>
       <c t="s" s="3" r="B64">
@@ -15119,7 +15119,7 @@
       </c>
     </row>
     <row r="65">
-      <c t="s" s="2" r="A65">
+      <c t="s" s="1" r="A65">
         <v>876</v>
       </c>
       <c t="s" s="3" r="B65">
@@ -15188,7 +15188,7 @@
       </c>
     </row>
     <row r="66">
-      <c t="s" s="2" r="A66">
+      <c t="s" s="1" r="A66">
         <v>895</v>
       </c>
       <c t="s" s="3" r="B66">
@@ -15255,7 +15255,7 @@
       </c>
     </row>
     <row r="67">
-      <c t="s" s="2" r="A67">
+      <c t="s" s="1" r="A67">
         <v>911</v>
       </c>
       <c t="s" s="3" r="B67">
@@ -15322,7 +15322,7 @@
       </c>
     </row>
     <row r="68">
-      <c t="s" s="2" r="A68">
+      <c t="s" s="1" r="A68">
         <v>923</v>
       </c>
       <c t="s" s="3" r="B68">
@@ -15389,7 +15389,7 @@
       </c>
     </row>
     <row r="69">
-      <c t="s" s="2" r="A69">
+      <c t="s" s="1" r="A69">
         <v>936</v>
       </c>
       <c t="s" s="3" r="B69">
@@ -15456,7 +15456,7 @@
       </c>
     </row>
     <row r="70">
-      <c t="s" s="2" r="A70">
+      <c t="s" s="1" r="A70">
         <v>950</v>
       </c>
       <c t="s" s="3" r="B70">
@@ -15525,7 +15525,7 @@
       </c>
     </row>
     <row r="71">
-      <c t="s" s="2" r="A71">
+      <c t="s" s="1" r="A71">
         <v>970</v>
       </c>
       <c t="s" s="3" r="B71">
@@ -15594,7 +15594,7 @@
       </c>
     </row>
     <row r="72">
-      <c t="s" s="2" r="A72">
+      <c t="s" s="1" r="A72">
         <v>986</v>
       </c>
       <c t="s" s="3" r="B72">
@@ -15659,7 +15659,7 @@
       </c>
     </row>
     <row r="73">
-      <c t="s" s="2" r="A73">
+      <c t="s" s="1" r="A73">
         <v>990</v>
       </c>
       <c t="s" s="3" r="B73">
@@ -15728,7 +15728,7 @@
       </c>
     </row>
     <row r="74">
-      <c t="s" s="2" r="A74">
+      <c t="s" s="1" r="A74">
         <v>1001</v>
       </c>
       <c t="s" s="3" r="B74">
@@ -15797,7 +15797,7 @@
       </c>
     </row>
     <row r="75">
-      <c t="s" s="2" r="A75">
+      <c t="s" s="1" r="A75">
         <v>1018</v>
       </c>
       <c t="s" s="3" r="B75">
@@ -15862,7 +15862,7 @@
       </c>
     </row>
     <row r="76">
-      <c t="s" s="2" r="A76">
+      <c t="s" s="1" r="A76">
         <v>1033</v>
       </c>
       <c t="s" s="3" r="B76">
@@ -15927,7 +15927,7 @@
       </c>
     </row>
     <row r="77">
-      <c t="s" s="2" r="A77">
+      <c t="s" s="1" r="A77">
         <v>1050</v>
       </c>
       <c t="s" s="3" r="B77">
@@ -15996,7 +15996,7 @@
       </c>
     </row>
     <row r="78">
-      <c t="s" s="2" r="A78">
+      <c t="s" s="1" r="A78">
         <v>1070</v>
       </c>
       <c t="s" s="3" r="B78">
@@ -16065,7 +16065,7 @@
       </c>
     </row>
     <row r="79">
-      <c t="s" s="2" r="A79">
+      <c t="s" s="1" r="A79">
         <v>1090</v>
       </c>
       <c t="s" s="3" r="B79">
@@ -16134,7 +16134,7 @@
       </c>
     </row>
     <row r="80">
-      <c t="s" s="2" r="A80">
+      <c t="s" s="1" r="A80">
         <v>1108</v>
       </c>
       <c t="s" s="3" r="B80">
@@ -16203,7 +16203,7 @@
       </c>
     </row>
     <row r="81">
-      <c t="s" s="2" r="A81">
+      <c t="s" s="1" r="A81">
         <v>1129</v>
       </c>
       <c t="s" s="3" r="B81">
@@ -16274,7 +16274,7 @@
       </c>
     </row>
     <row r="82">
-      <c t="s" s="2" r="A82">
+      <c t="s" s="1" r="A82">
         <v>1150</v>
       </c>
       <c t="s" s="3" r="B82">
@@ -16345,7 +16345,7 @@
       </c>
     </row>
     <row r="83">
-      <c t="s" s="2" r="A83">
+      <c t="s" s="1" r="A83">
         <v>1171</v>
       </c>
       <c t="s" s="3" r="B83">
@@ -16416,7 +16416,7 @@
       </c>
     </row>
     <row r="84">
-      <c t="s" s="2" r="A84">
+      <c t="s" s="1" r="A84">
         <v>1192</v>
       </c>
       <c t="s" s="3" r="B84">
@@ -16485,7 +16485,7 @@
       </c>
     </row>
     <row r="85">
-      <c t="s" s="2" r="A85">
+      <c t="s" s="1" r="A85">
         <v>1194</v>
       </c>
       <c t="s" s="3" r="B85">
@@ -16554,7 +16554,7 @@
       </c>
     </row>
     <row r="86">
-      <c t="s" s="2" r="A86">
+      <c t="s" s="1" r="A86">
         <v>1196</v>
       </c>
       <c t="s" s="3" r="B86">
@@ -16623,7 +16623,7 @@
       </c>
     </row>
     <row r="87">
-      <c t="s" s="2" r="A87">
+      <c t="s" s="1" r="A87">
         <v>1198</v>
       </c>
       <c t="s" s="3" r="B87">
@@ -16692,7 +16692,7 @@
       </c>
     </row>
     <row r="88">
-      <c t="s" s="2" r="A88">
+      <c t="s" s="1" r="A88">
         <v>1218</v>
       </c>
       <c t="s" s="3" r="B88">
@@ -16761,7 +16761,7 @@
       </c>
     </row>
     <row r="89">
-      <c t="s" s="2" r="A89">
+      <c t="s" s="1" r="A89">
         <v>1238</v>
       </c>
       <c t="s" s="3" r="B89">
@@ -16832,7 +16832,7 @@
       </c>
     </row>
     <row r="90">
-      <c t="s" s="2" r="A90">
+      <c t="s" s="1" r="A90">
         <v>1259</v>
       </c>
       <c t="s" s="3" r="B90">
@@ -16905,7 +16905,7 @@
       </c>
     </row>
     <row r="91">
-      <c t="s" s="2" r="A91">
+      <c t="s" s="1" r="A91">
         <v>1281</v>
       </c>
       <c t="s" s="3" r="B91">
@@ -16978,7 +16978,7 @@
       </c>
     </row>
     <row r="92">
-      <c t="s" s="2" r="A92">
+      <c t="s" s="1" r="A92">
         <v>1303</v>
       </c>
       <c t="s" s="3" r="B92">
@@ -17051,7 +17051,7 @@
       </c>
     </row>
     <row r="93">
-      <c t="s" s="2" r="A93">
+      <c t="s" s="1" r="A93">
         <v>1326</v>
       </c>
       <c t="s" s="3" r="B93">
@@ -17124,7 +17124,7 @@
       </c>
     </row>
     <row r="94">
-      <c t="s" s="2" r="A94">
+      <c t="s" s="1" r="A94">
         <v>1348</v>
       </c>
       <c t="s" s="3" r="B94">
@@ -17197,7 +17197,7 @@
       </c>
     </row>
     <row r="95">
-      <c t="s" s="2" r="A95">
+      <c t="s" s="1" r="A95">
         <v>1370</v>
       </c>
       <c t="s" s="3" r="B95">
@@ -17270,7 +17270,7 @@
       </c>
     </row>
     <row r="96">
-      <c t="s" s="2" r="A96">
+      <c t="s" s="1" r="A96">
         <v>1391</v>
       </c>
       <c t="s" s="3" r="B96">
@@ -17343,7 +17343,7 @@
       </c>
     </row>
     <row r="97">
-      <c t="s" s="2" r="A97">
+      <c t="s" s="1" r="A97">
         <v>1398</v>
       </c>
       <c t="s" s="3" r="B97">
@@ -17416,7 +17416,7 @@
       </c>
     </row>
     <row r="98">
-      <c t="s" s="2" r="A98">
+      <c t="s" s="1" r="A98">
         <v>1419</v>
       </c>
       <c t="s" s="3" r="B98">
@@ -17489,7 +17489,7 @@
       </c>
     </row>
     <row r="99">
-      <c t="s" s="2" r="A99">
+      <c t="s" s="1" r="A99">
         <v>1440</v>
       </c>
       <c t="s" s="3" r="B99">
@@ -17562,7 +17562,7 @@
       </c>
     </row>
     <row r="100">
-      <c t="s" s="2" r="A100">
+      <c t="s" s="1" r="A100">
         <v>1462</v>
       </c>
       <c t="s" s="3" r="B100">
@@ -17635,7 +17635,7 @@
       </c>
     </row>
     <row r="101">
-      <c t="s" s="2" r="A101">
+      <c t="s" s="1" r="A101">
         <v>1485</v>
       </c>
       <c t="s" s="3" r="B101">
@@ -17708,7 +17708,7 @@
       </c>
     </row>
     <row r="102">
-      <c t="s" s="2" r="A102">
+      <c t="s" s="1" r="A102">
         <v>1507</v>
       </c>
       <c t="s" s="3" r="B102">
@@ -17781,7 +17781,7 @@
       </c>
     </row>
     <row r="103">
-      <c t="s" s="2" r="A103">
+      <c t="s" s="1" r="A103">
         <v>1530</v>
       </c>
       <c t="s" s="3" r="B103">
@@ -17854,7 +17854,7 @@
       </c>
     </row>
     <row r="104">
-      <c t="s" s="2" r="A104">
+      <c t="s" s="1" r="A104">
         <v>1552</v>
       </c>
       <c t="s" s="3" r="B104">
@@ -17927,7 +17927,7 @@
       </c>
     </row>
     <row r="105">
-      <c t="s" s="2" r="A105">
+      <c t="s" s="1" r="A105">
         <v>1575</v>
       </c>
       <c t="s" s="3" r="B105">
@@ -18000,7 +18000,7 @@
       </c>
     </row>
     <row r="106">
-      <c t="s" s="2" r="A106">
+      <c t="s" s="1" r="A106">
         <v>1598</v>
       </c>
       <c t="s" s="3" r="B106">
@@ -18073,7 +18073,7 @@
       </c>
     </row>
     <row r="107">
-      <c t="s" s="2" r="A107">
+      <c t="s" s="1" r="A107">
         <v>1611</v>
       </c>
       <c t="s" s="3" r="B107">
@@ -18146,7 +18146,7 @@
       </c>
     </row>
     <row r="108">
-      <c t="s" s="2" r="A108">
+      <c t="s" s="1" r="A108">
         <v>1630</v>
       </c>
       <c t="s" s="3" r="B108">
@@ -18217,7 +18217,7 @@
       </c>
     </row>
     <row r="109">
-      <c t="s" s="2" r="A109">
+      <c t="s" s="1" r="A109">
         <v>1634</v>
       </c>
       <c t="s" s="3" r="B109">
@@ -18288,7 +18288,7 @@
       </c>
     </row>
     <row r="110">
-      <c t="s" s="2" r="A110">
+      <c t="s" s="1" r="A110">
         <v>1637</v>
       </c>
       <c t="s" s="3" r="B110">
@@ -18361,7 +18361,7 @@
       </c>
     </row>
     <row r="111">
-      <c t="s" s="2" r="A111">
+      <c t="s" s="1" r="A111">
         <v>1658</v>
       </c>
       <c t="s" s="3" r="B111">
@@ -18434,7 +18434,7 @@
       </c>
     </row>
     <row r="112">
-      <c t="s" s="2" r="A112">
+      <c t="s" s="1" r="A112">
         <v>1667</v>
       </c>
       <c t="s" s="3" r="B112">
@@ -18507,7 +18507,7 @@
       </c>
     </row>
     <row r="113">
-      <c t="s" s="2" r="A113">
+      <c t="s" s="1" r="A113">
         <v>1689</v>
       </c>
       <c t="s" s="3" r="B113">
@@ -18580,7 +18580,7 @@
       </c>
     </row>
     <row r="114">
-      <c t="s" s="2" r="A114">
+      <c t="s" s="1" r="A114">
         <v>1709</v>
       </c>
       <c t="s" s="3" r="B114">
@@ -18653,7 +18653,7 @@
       </c>
     </row>
     <row r="115">
-      <c t="s" s="2" r="A115">
+      <c t="s" s="1" r="A115">
         <v>1730</v>
       </c>
       <c t="s" s="3" r="B115">
@@ -18730,7 +18730,7 @@
       </c>
     </row>
     <row r="116">
-      <c t="s" s="2" r="A116">
+      <c t="s" s="1" r="A116">
         <v>1733</v>
       </c>
       <c t="s" s="3" r="B116">
@@ -18807,7 +18807,7 @@
       </c>
     </row>
     <row r="117">
-      <c t="s" s="2" r="A117">
+      <c t="s" s="1" r="A117">
         <v>1756</v>
       </c>
       <c t="s" s="3" r="B117">
@@ -18884,7 +18884,7 @@
       </c>
     </row>
     <row r="118">
-      <c t="s" s="2" r="A118">
+      <c t="s" s="1" r="A118">
         <v>1775</v>
       </c>
       <c t="s" s="3" r="B118">
@@ -18959,7 +18959,7 @@
       </c>
     </row>
     <row r="119">
-      <c t="s" s="2" r="A119">
+      <c t="s" s="1" r="A119">
         <v>1793</v>
       </c>
       <c t="s" s="3" r="B119">
@@ -19036,7 +19036,7 @@
       </c>
     </row>
     <row r="120">
-      <c t="s" s="2" r="A120">
+      <c t="s" s="1" r="A120">
         <v>1818</v>
       </c>
       <c t="s" s="3" r="B120">
@@ -19113,7 +19113,7 @@
       </c>
     </row>
     <row r="121">
-      <c t="s" s="2" r="A121">
+      <c t="s" s="1" r="A121">
         <v>1842</v>
       </c>
       <c t="s" s="3" r="B121">
@@ -19190,7 +19190,7 @@
       </c>
     </row>
     <row r="122">
-      <c t="s" s="2" r="A122">
+      <c t="s" s="1" r="A122">
         <v>1864</v>
       </c>
       <c t="s" s="3" r="B122">
@@ -19265,7 +19265,7 @@
       </c>
     </row>
     <row r="123">
-      <c t="s" s="2" r="A123">
+      <c t="s" s="1" r="A123">
         <v>1885</v>
       </c>
       <c t="s" s="3" r="B123">
@@ -19342,7 +19342,7 @@
       </c>
     </row>
     <row r="124">
-      <c t="s" s="2" r="A124">
+      <c t="s" s="1" r="A124">
         <v>1909</v>
       </c>
       <c t="s" s="3" r="B124">
@@ -19417,7 +19417,7 @@
       </c>
     </row>
     <row r="125">
-      <c t="s" s="2" r="A125">
+      <c t="s" s="1" r="A125">
         <v>1933</v>
       </c>
       <c t="s" s="3" r="B125">
@@ -19492,7 +19492,7 @@
       </c>
     </row>
     <row r="126">
-      <c t="s" s="2" r="A126">
+      <c t="s" s="1" r="A126">
         <v>1949</v>
       </c>
       <c t="s" s="3" r="B126">
@@ -19567,7 +19567,7 @@
       </c>
     </row>
     <row r="127">
-      <c t="s" s="2" r="A127">
+      <c t="s" s="1" r="A127">
         <v>1966</v>
       </c>
       <c t="s" s="3" r="B127">
@@ -19644,7 +19644,7 @@
       </c>
     </row>
     <row r="128">
-      <c t="s" s="2" r="A128">
+      <c t="s" s="1" r="A128">
         <v>1989</v>
       </c>
       <c t="s" s="3" r="B128">
@@ -19719,7 +19719,7 @@
       </c>
     </row>
     <row r="129">
-      <c t="s" s="2" r="A129">
+      <c t="s" s="1" r="A129">
         <v>2007</v>
       </c>
       <c t="s" s="3" r="B129">
@@ -19796,7 +19796,7 @@
       </c>
     </row>
     <row r="130">
-      <c t="s" s="2" r="A130">
+      <c t="s" s="1" r="A130">
         <v>2032</v>
       </c>
       <c t="s" s="3" r="B130">
@@ -19871,7 +19871,7 @@
       </c>
     </row>
     <row r="131">
-      <c t="s" s="2" r="A131">
+      <c t="s" s="1" r="A131">
         <v>2049</v>
       </c>
       <c t="s" s="3" r="B131">
@@ -19946,7 +19946,7 @@
       </c>
     </row>
     <row r="132">
-      <c t="s" s="2" r="A132">
+      <c t="s" s="1" r="A132">
         <v>2065</v>
       </c>
       <c t="s" s="3" r="B132">
@@ -20021,7 +20021,7 @@
       </c>
     </row>
     <row r="133">
-      <c t="s" s="2" r="A133">
+      <c t="s" s="1" r="A133">
         <v>2089</v>
       </c>
       <c t="s" s="3" r="B133">
@@ -20098,7 +20098,7 @@
       </c>
     </row>
     <row r="134">
-      <c t="s" s="2" r="A134">
+      <c t="s" s="1" r="A134">
         <v>2114</v>
       </c>
       <c t="s" s="3" r="B134">
@@ -20175,7 +20175,7 @@
       </c>
     </row>
     <row r="135">
-      <c t="s" s="2" r="A135">
+      <c t="s" s="1" r="A135">
         <v>2139</v>
       </c>
       <c t="s" s="3" r="B135">
@@ -20250,7 +20250,7 @@
       </c>
     </row>
     <row r="136">
-      <c t="s" s="2" r="A136">
+      <c t="s" s="1" r="A136">
         <v>2163</v>
       </c>
       <c t="s" s="3" r="B136">
@@ -20325,7 +20325,7 @@
       </c>
     </row>
     <row r="137">
-      <c t="s" s="2" r="A137">
+      <c t="s" s="1" r="A137">
         <v>2186</v>
       </c>
       <c t="s" s="3" r="B137">
@@ -20400,7 +20400,7 @@
       </c>
     </row>
     <row r="138">
-      <c t="s" s="2" r="A138">
+      <c t="s" s="1" r="A138">
         <v>2209</v>
       </c>
       <c t="s" s="3" r="B138">
@@ -20477,7 +20477,7 @@
       </c>
     </row>
     <row r="139">
-      <c t="s" s="2" r="A139">
+      <c t="s" s="1" r="A139">
         <v>2219</v>
       </c>
       <c t="s" s="3" r="B139">
@@ -20552,7 +20552,7 @@
       </c>
     </row>
     <row r="140">
-      <c t="s" s="2" r="A140">
+      <c t="s" s="1" r="A140">
         <v>2242</v>
       </c>
       <c t="s" s="3" r="B140">
@@ -20629,7 +20629,7 @@
       </c>
     </row>
     <row r="141">
-      <c t="s" s="2" r="A141">
+      <c t="s" s="1" r="A141">
         <v>2266</v>
       </c>
       <c t="s" s="3" r="B141">
@@ -20704,7 +20704,7 @@
       </c>
     </row>
     <row r="142">
-      <c t="s" s="2" r="A142">
+      <c t="s" s="1" r="A142">
         <v>2290</v>
       </c>
       <c t="s" s="3" r="B142">
@@ -20781,7 +20781,7 @@
       </c>
     </row>
     <row r="143">
-      <c t="s" s="2" r="A143">
+      <c t="s" s="1" r="A143">
         <v>2303</v>
       </c>
       <c t="s" s="3" r="B143">
@@ -20856,7 +20856,7 @@
       </c>
     </row>
     <row r="144">
-      <c t="s" s="2" r="A144">
+      <c t="s" s="1" r="A144">
         <v>2306</v>
       </c>
       <c t="s" s="3" r="B144">
@@ -20933,7 +20933,7 @@
       </c>
     </row>
     <row r="145">
-      <c t="s" s="2" r="A145">
+      <c t="s" s="1" r="A145">
         <v>2309</v>
       </c>
       <c t="s" s="3" r="B145">
@@ -21010,7 +21010,7 @@
       </c>
     </row>
     <row r="146">
-      <c t="s" s="2" r="A146">
+      <c t="s" s="1" r="A146">
         <v>2312</v>
       </c>
       <c t="s" s="3" r="B146">
@@ -21087,7 +21087,7 @@
       </c>
     </row>
     <row r="147">
-      <c t="s" s="2" r="A147">
+      <c t="s" s="1" r="A147">
         <v>2315</v>
       </c>
       <c t="s" s="3" r="B147">
@@ -21164,7 +21164,7 @@
       </c>
     </row>
     <row r="148">
-      <c t="s" s="2" r="A148">
+      <c t="s" s="1" r="A148">
         <v>2338</v>
       </c>
       <c t="s" s="3" r="B148">
@@ -21239,7 +21239,7 @@
       </c>
     </row>
     <row r="149">
-      <c t="s" s="2" r="A149">
+      <c t="s" s="1" r="A149">
         <v>2362</v>
       </c>
       <c t="s" s="3" r="B149">
@@ -21316,7 +21316,7 @@
       </c>
     </row>
     <row r="150">
-      <c t="s" s="2" r="A150">
+      <c t="s" s="1" r="A150">
         <v>2387</v>
       </c>
       <c t="s" s="3" r="B150">
@@ -21393,7 +21393,7 @@
       </c>
     </row>
     <row r="151">
-      <c t="s" s="2" r="A151">
+      <c t="s" s="1" r="A151">
         <v>2412</v>
       </c>
       <c t="s" s="3" r="B151">
@@ -21470,7 +21470,7 @@
       </c>
     </row>
     <row r="152">
-      <c t="s" s="2" r="A152">
+      <c t="s" s="1" r="A152">
         <v>2437</v>
       </c>
       <c t="s" s="3" r="B152">
@@ -21545,7 +21545,7 @@
       </c>
     </row>
     <row r="153">
-      <c t="s" s="2" r="A153">
+      <c t="s" s="1" r="A153">
         <v>2461</v>
       </c>
       <c t="s" s="3" r="B153">
@@ -21622,7 +21622,7 @@
       </c>
     </row>
     <row r="154">
-      <c t="s" s="2" r="A154">
+      <c t="s" s="1" r="A154">
         <v>2486</v>
       </c>
       <c t="s" s="3" r="B154">
@@ -21699,7 +21699,7 @@
       </c>
     </row>
     <row r="155">
-      <c t="s" s="2" r="A155">
+      <c t="s" s="1" r="A155">
         <v>2510</v>
       </c>
       <c t="s" s="3" r="B155">
@@ -21776,7 +21776,7 @@
       </c>
     </row>
     <row r="156">
-      <c t="s" s="2" r="A156">
+      <c t="s" s="1" r="A156">
         <v>2522</v>
       </c>
       <c t="s" s="3" r="B156">
@@ -21851,7 +21851,7 @@
       </c>
     </row>
     <row r="157">
-      <c t="s" s="2" r="A157">
+      <c t="s" s="1" r="A157">
         <v>2534</v>
       </c>
       <c t="s" s="3" r="B157">
@@ -21926,7 +21926,7 @@
       </c>
     </row>
     <row r="158">
-      <c t="s" s="2" r="A158">
+      <c t="s" s="1" r="A158">
         <v>2539</v>
       </c>
       <c t="s" s="3" r="B158">
@@ -22003,7 +22003,7 @@
       </c>
     </row>
     <row r="159">
-      <c t="s" s="2" r="A159">
+      <c t="s" s="1" r="A159">
         <v>2562</v>
       </c>
       <c t="s" s="3" r="B159">
@@ -22078,7 +22078,7 @@
       </c>
     </row>
     <row r="160">
-      <c t="s" s="2" r="A160">
+      <c t="s" s="1" r="A160">
         <v>2577</v>
       </c>
       <c t="s" s="3" r="B160">
@@ -22153,7 +22153,7 @@
       </c>
     </row>
     <row r="161">
-      <c t="s" s="2" r="A161">
+      <c t="s" s="1" r="A161">
         <v>2601</v>
       </c>
       <c t="s" s="3" r="B161">
@@ -22228,7 +22228,7 @@
       </c>
     </row>
     <row r="162">
-      <c t="s" s="2" r="A162">
+      <c t="s" s="1" r="A162">
         <v>2622</v>
       </c>
       <c t="s" s="3" r="B162">
@@ -22303,7 +22303,7 @@
       </c>
     </row>
     <row r="163">
-      <c t="s" s="2" r="A163">
+      <c t="s" s="1" r="A163">
         <v>2646</v>
       </c>
       <c t="s" s="3" r="B163">
@@ -22378,7 +22378,7 @@
       </c>
     </row>
     <row r="164">
-      <c t="s" s="2" r="A164">
+      <c t="s" s="1" r="A164">
         <v>2661</v>
       </c>
       <c t="s" s="3" r="B164">
@@ -22449,7 +22449,7 @@
       </c>
     </row>
     <row r="165">
-      <c t="s" s="2" r="A165">
+      <c t="s" s="1" r="A165">
         <v>2664</v>
       </c>
       <c t="s" s="3" r="B165">
@@ -22520,7 +22520,7 @@
       </c>
     </row>
     <row r="166">
-      <c t="s" s="2" r="A166">
+      <c t="s" s="1" r="A166">
         <v>2667</v>
       </c>
       <c t="s" s="3" r="B166">
@@ -22591,7 +22591,7 @@
       </c>
     </row>
     <row r="167">
-      <c t="s" s="2" r="A167">
+      <c t="s" s="1" r="A167">
         <v>2670</v>
       </c>
       <c t="s" s="3" r="B167">
@@ -22666,153 +22666,153 @@
       </c>
     </row>
     <row r="168">
-      <c t="s" s="2" r="A168">
+      <c t="s" s="1" r="A168">
         <v>2677</v>
       </c>
-      <c t="s" s="1" r="B168">
+      <c t="s" s="2" r="B168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="C168">
+      <c t="s" s="2" r="C168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="D168">
+      <c t="s" s="2" r="D168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="E168">
+      <c t="s" s="2" r="E168">
         <v>2678</v>
       </c>
       <c t="s" s="3" r="F168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="G168">
+      <c t="s" s="2" r="G168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="H168">
+      <c t="s" s="2" r="H168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="I168">
+      <c t="s" s="2" r="I168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="J168">
+      <c t="s" s="2" r="J168">
         <v>2679</v>
       </c>
-      <c t="s" s="1" r="K168">
+      <c t="s" s="2" r="K168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="L168">
+      <c t="s" s="2" r="L168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="M168">
+      <c t="s" s="2" r="M168">
         <v>2678</v>
       </c>
       <c t="s" s="3" r="N168">
         <v>2678</v>
       </c>
       <c s="3" r="O168"/>
-      <c t="s" s="1" r="P168">
+      <c t="s" s="2" r="P168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="Q168">
+      <c t="s" s="2" r="Q168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="R168">
+      <c t="s" s="2" r="R168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="S168">
+      <c t="s" s="2" r="S168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="T168">
+      <c t="s" s="2" r="T168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="U168">
+      <c t="s" s="2" r="U168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="V168">
+      <c t="s" s="2" r="V168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="W168">
+      <c t="s" s="2" r="W168">
         <v>2678</v>
       </c>
       <c t="s" s="3" r="X168">
         <v>2678</v>
       </c>
-      <c t="s" s="1" r="Y168">
+      <c t="s" s="2" r="Y168">
         <v>2678</v>
       </c>
     </row>
     <row r="169">
-      <c t="s" s="2" r="A169">
+      <c t="s" s="1" r="A169">
         <v>2680</v>
       </c>
-      <c t="s" s="1" r="B169">
+      <c t="s" s="2" r="B169">
         <v>2681</v>
       </c>
-      <c t="s" s="1" r="C169">
+      <c t="s" s="2" r="C169">
         <v>2681</v>
       </c>
-      <c t="s" s="1" r="D169">
+      <c t="s" s="2" r="D169">
         <v>2681</v>
       </c>
-      <c t="s" s="1" r="E169">
+      <c t="s" s="2" r="E169">
         <v>2681</v>
       </c>
       <c t="s" s="3" r="F169">
         <v>2681</v>
       </c>
-      <c t="s" s="1" r="G169">
+      <c t="s" s="2" r="G169">
         <v>2681</v>
       </c>
       <c s="3" r="H169"/>
-      <c t="s" s="1" r="I169">
+      <c t="s" s="2" r="I169">
         <v>2681</v>
       </c>
       <c t="s" s="3" r="J169">
         <v>2682</v>
       </c>
-      <c t="s" s="1" r="K169">
+      <c t="s" s="2" r="K169">
         <v>2681</v>
       </c>
-      <c t="s" s="1" r="L169">
+      <c t="s" s="2" r="L169">
         <v>2681</v>
       </c>
-      <c t="s" s="1" r="M169">
+      <c t="s" s="2" r="M169">
         <v>2681</v>
       </c>
       <c s="3" r="N169"/>
       <c s="3" r="O169"/>
-      <c t="s" s="1" r="P169">
+      <c t="s" s="2" r="P169">
         <v>2681</v>
       </c>
-      <c t="s" s="1" r="Q169">
+      <c t="s" s="2" r="Q169">
         <v>2681</v>
       </c>
-      <c t="s" s="1" r="R169">
+      <c t="s" s="2" r="R169">
         <v>2683</v>
       </c>
-      <c t="s" s="1" r="S169">
+      <c t="s" s="2" r="S169">
         <v>2681</v>
       </c>
-      <c t="s" s="1" r="T169">
+      <c t="s" s="2" r="T169">
         <v>2684</v>
       </c>
-      <c t="s" s="1" r="U169">
+      <c t="s" s="2" r="U169">
         <v>2681</v>
       </c>
-      <c t="s" s="1" r="V169">
+      <c t="s" s="2" r="V169">
         <v>2681</v>
       </c>
-      <c t="s" s="1" r="W169">
+      <c t="s" s="2" r="W169">
         <v>2681</v>
       </c>
       <c t="s" s="3" r="X169">
         <v>2681</v>
       </c>
-      <c t="s" s="1" r="Y169">
+      <c t="s" s="2" r="Y169">
         <v>2681</v>
       </c>
     </row>
     <row r="170">
-      <c t="s" s="2" r="A170">
+      <c t="s" s="1" r="A170">
         <v>2685</v>
       </c>
       <c t="s" s="3" r="B170">
@@ -22883,7 +22883,7 @@
       </c>
     </row>
     <row r="171">
-      <c t="s" s="2" r="A171">
+      <c t="s" s="1" r="A171">
         <v>2688</v>
       </c>
       <c t="s" s="3" r="B171">
@@ -22954,7 +22954,7 @@
       </c>
     </row>
     <row r="172">
-      <c t="s" s="2" r="A172">
+      <c t="s" s="1" r="A172">
         <v>2691</v>
       </c>
       <c t="s" s="3" r="B172">
@@ -23025,100 +23025,100 @@
       </c>
     </row>
     <row r="173">
-      <c t="s" s="2" r="A173">
+      <c t="s" s="1" r="A173">
         <v>2694</v>
       </c>
-      <c t="s" s="1" r="B173">
+      <c t="s" s="2" r="B173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="C173">
+      <c t="s" s="2" r="C173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="D173">
+      <c t="s" s="2" r="D173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="E173">
+      <c t="s" s="2" r="E173">
         <v>2695</v>
       </c>
       <c t="s" s="3" r="F173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="G173">
+      <c t="s" s="2" r="G173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="H173">
+      <c t="s" s="2" r="H173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="I173">
+      <c t="s" s="2" r="I173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="J173">
+      <c t="s" s="2" r="J173">
         <v>2696</v>
       </c>
-      <c t="s" s="1" r="K173">
+      <c t="s" s="2" r="K173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="L173">
+      <c t="s" s="2" r="L173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="M173">
+      <c t="s" s="2" r="M173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="N173">
+      <c t="s" s="2" r="N173">
         <v>2697</v>
       </c>
       <c s="3" r="O173"/>
-      <c t="s" s="1" r="P173">
+      <c t="s" s="2" r="P173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="Q173">
+      <c t="s" s="2" r="Q173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="R173">
+      <c t="s" s="2" r="R173">
         <v>2698</v>
       </c>
-      <c t="s" s="1" r="S173">
+      <c t="s" s="2" r="S173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="T173">
+      <c t="s" s="2" r="T173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="U173">
+      <c t="s" s="2" r="U173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="V173">
+      <c t="s" s="2" r="V173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="W173">
+      <c t="s" s="2" r="W173">
         <v>2695</v>
       </c>
       <c t="s" s="3" r="X173">
         <v>2695</v>
       </c>
-      <c t="s" s="1" r="Y173">
+      <c t="s" s="2" r="Y173">
         <v>2695</v>
       </c>
     </row>
     <row r="174">
-      <c t="s" s="2" r="A174">
+      <c t="s" s="1" r="A174">
         <v>2699</v>
       </c>
-      <c t="s" s="1" r="B174">
+      <c t="s" s="2" r="B174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="C174">
+      <c t="s" s="2" r="C174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="D174">
+      <c t="s" s="2" r="D174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="E174">
+      <c t="s" s="2" r="E174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="F174">
+      <c t="s" s="2" r="F174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="G174">
+      <c t="s" s="2" r="G174">
         <v>2700</v>
       </c>
       <c s="3" r="H174"/>
@@ -23126,50 +23126,50 @@
       <c t="s" s="3" r="J174">
         <v>2701</v>
       </c>
-      <c t="s" s="1" r="K174">
+      <c t="s" s="2" r="K174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="L174">
+      <c t="s" s="2" r="L174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="M174">
+      <c t="s" s="2" r="M174">
         <v>2700</v>
       </c>
       <c s="3" r="N174"/>
       <c s="3" r="O174"/>
-      <c t="s" s="1" r="P174">
+      <c t="s" s="2" r="P174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="Q174">
+      <c t="s" s="2" r="Q174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="R174">
+      <c t="s" s="2" r="R174">
         <v>2698</v>
       </c>
-      <c t="s" s="1" r="S174">
+      <c t="s" s="2" r="S174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="T174">
+      <c t="s" s="2" r="T174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="U174">
+      <c t="s" s="2" r="U174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="V174">
+      <c t="s" s="2" r="V174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="W174">
+      <c t="s" s="2" r="W174">
         <v>2700</v>
       </c>
       <c t="s" s="3" r="X174">
         <v>2700</v>
       </c>
-      <c t="s" s="1" r="Y174">
+      <c t="s" s="2" r="Y174">
         <v>2700</v>
       </c>
     </row>
     <row r="175">
-      <c t="s" s="2" r="A175">
+      <c t="s" s="1" r="A175">
         <v>2702</v>
       </c>
       <c t="s" s="3" r="B175">
@@ -23246,7 +23246,7 @@
       </c>
     </row>
     <row r="176">
-      <c t="s" s="2" r="A176">
+      <c t="s" s="1" r="A176">
         <v>2726</v>
       </c>
       <c t="s" s="3" r="B176">
@@ -23321,7 +23321,7 @@
       </c>
     </row>
     <row r="177">
-      <c t="s" s="2" r="A177">
+      <c t="s" s="1" r="A177">
         <v>2746</v>
       </c>
       <c t="s" s="3" r="B177">
@@ -23396,7 +23396,7 @@
       </c>
     </row>
     <row r="178">
-      <c t="s" s="2" r="A178">
+      <c t="s" s="1" r="A178">
         <v>2749</v>
       </c>
       <c t="s" s="3" r="B178">
@@ -23471,7 +23471,7 @@
       </c>
     </row>
     <row r="179">
-      <c t="s" s="2" r="A179">
+      <c t="s" s="1" r="A179">
         <v>2754</v>
       </c>
       <c t="s" s="3" r="B179">
@@ -23546,7 +23546,7 @@
       </c>
     </row>
     <row r="180">
-      <c t="s" s="2" r="A180">
+      <c t="s" s="1" r="A180">
         <v>2759</v>
       </c>
       <c t="s" s="3" r="B180">
@@ -23621,7 +23621,7 @@
       </c>
     </row>
     <row r="181">
-      <c t="s" s="2" r="A181">
+      <c t="s" s="1" r="A181">
         <v>2763</v>
       </c>
       <c t="s" s="3" r="B181">
@@ -23696,7 +23696,7 @@
       </c>
     </row>
     <row r="182">
-      <c t="s" s="2" r="A182">
+      <c t="s" s="1" r="A182">
         <v>2766</v>
       </c>
       <c t="s" s="3" r="B182">
@@ -23771,7 +23771,7 @@
       </c>
     </row>
     <row r="183">
-      <c t="s" s="2" r="A183">
+      <c t="s" s="1" r="A183">
         <v>2770</v>
       </c>
       <c t="s" s="3" r="B183">
@@ -23846,7 +23846,7 @@
       </c>
     </row>
     <row r="184">
-      <c t="s" s="2" r="A184">
+      <c t="s" s="1" r="A184">
         <v>2773</v>
       </c>
       <c t="s" s="3" r="B184">
@@ -23921,7 +23921,7 @@
       </c>
     </row>
     <row r="185">
-      <c t="s" s="2" r="A185">
+      <c t="s" s="1" r="A185">
         <v>2776</v>
       </c>
       <c t="s" s="3" r="B185">
@@ -23996,7 +23996,7 @@
       </c>
     </row>
     <row r="186">
-      <c t="s" s="2" r="A186">
+      <c t="s" s="1" r="A186">
         <v>2796</v>
       </c>
       <c t="s" s="3" r="B186">
@@ -24071,7 +24071,7 @@
       </c>
     </row>
     <row r="187">
-      <c t="s" s="2" r="A187">
+      <c t="s" s="1" r="A187">
         <v>2819</v>
       </c>
       <c t="s" s="3" r="B187">
@@ -24148,7 +24148,7 @@
       </c>
     </row>
     <row r="188">
-      <c t="s" s="2" r="A188">
+      <c t="s" s="1" r="A188">
         <v>2828</v>
       </c>
       <c t="s" s="3" r="B188">
@@ -24225,7 +24225,7 @@
       </c>
     </row>
     <row r="189">
-      <c t="s" s="2" r="A189">
+      <c t="s" s="1" r="A189">
         <v>2836</v>
       </c>
       <c t="s" s="3" r="B189">
@@ -24300,7 +24300,7 @@
       </c>
     </row>
     <row r="190">
-      <c t="s" s="2" r="A190">
+      <c t="s" s="1" r="A190">
         <v>2857</v>
       </c>
       <c t="s" s="3" r="B190">
@@ -24375,7 +24375,7 @@
       </c>
     </row>
     <row r="191">
-      <c t="s" s="2" r="A191">
+      <c t="s" s="1" r="A191">
         <v>2881</v>
       </c>
       <c t="s" s="3" r="B191">
@@ -24450,7 +24450,7 @@
       </c>
     </row>
     <row r="192">
-      <c t="s" s="2" r="A192">
+      <c t="s" s="1" r="A192">
         <v>2902</v>
       </c>
       <c t="s" s="3" r="B192">
@@ -24525,7 +24525,7 @@
       </c>
     </row>
     <row r="193">
-      <c t="s" s="2" r="A193">
+      <c t="s" s="1" r="A193">
         <v>2925</v>
       </c>
       <c t="s" s="3" r="B193">
@@ -24600,7 +24600,7 @@
       </c>
     </row>
     <row r="194">
-      <c t="s" s="2" r="A194">
+      <c t="s" s="1" r="A194">
         <v>2948</v>
       </c>
       <c t="s" s="3" r="B194">
@@ -24677,7 +24677,7 @@
       </c>
     </row>
     <row r="195">
-      <c t="s" s="2" r="A195">
+      <c t="s" s="1" r="A195">
         <v>2973</v>
       </c>
       <c t="s" s="3" r="B195">
@@ -24752,7 +24752,7 @@
       </c>
     </row>
     <row r="196">
-      <c t="s" s="2" r="A196">
+      <c t="s" s="1" r="A196">
         <v>2981</v>
       </c>
       <c t="s" s="3" r="B196">
@@ -24829,7 +24829,7 @@
       </c>
     </row>
     <row r="197">
-      <c t="s" s="2" r="A197">
+      <c t="s" s="1" r="A197">
         <v>3006</v>
       </c>
       <c t="s" s="3" r="B197">
@@ -24904,7 +24904,7 @@
       </c>
     </row>
     <row r="198">
-      <c t="s" s="2" r="A198">
+      <c t="s" s="1" r="A198">
         <v>3024</v>
       </c>
       <c t="s" s="3" r="B198">
@@ -24981,7 +24981,7 @@
       </c>
     </row>
     <row r="199">
-      <c t="s" s="2" r="A199">
+      <c t="s" s="1" r="A199">
         <v>3047</v>
       </c>
       <c t="s" s="3" r="B199">
@@ -25052,7 +25052,7 @@
       </c>
     </row>
     <row r="200">
-      <c t="s" s="2" r="A200">
+      <c t="s" s="1" r="A200">
         <v>3062</v>
       </c>
       <c t="s" s="3" r="B200">
@@ -25129,7 +25129,7 @@
       </c>
     </row>
     <row r="201">
-      <c t="s" s="2" r="A201">
+      <c t="s" s="1" r="A201">
         <v>3078</v>
       </c>
       <c t="s" s="3" r="B201">
@@ -25206,7 +25206,7 @@
       </c>
     </row>
     <row r="202">
-      <c t="s" s="2" r="A202">
+      <c t="s" s="1" r="A202">
         <v>3085</v>
       </c>
       <c t="s" s="3" r="B202">
@@ -25277,7 +25277,7 @@
       </c>
     </row>
     <row r="203">
-      <c t="s" s="2" r="A203">
+      <c t="s" s="1" r="A203">
         <v>3106</v>
       </c>
       <c t="s" s="3" r="B203">
@@ -25354,7 +25354,7 @@
       </c>
     </row>
     <row r="204">
-      <c t="s" s="2" r="A204">
+      <c t="s" s="1" r="A204">
         <v>3127</v>
       </c>
       <c t="s" s="3" r="B204">
@@ -25427,7 +25427,7 @@
       </c>
     </row>
     <row r="205">
-      <c t="s" s="2" r="A205">
+      <c t="s" s="1" r="A205">
         <v>3148</v>
       </c>
       <c t="s" s="3" r="B205">
@@ -25504,7 +25504,7 @@
       </c>
     </row>
     <row r="206">
-      <c t="s" s="2" r="A206">
+      <c t="s" s="1" r="A206">
         <v>3159</v>
       </c>
       <c t="s" s="3" r="B206">
@@ -25579,7 +25579,7 @@
       </c>
     </row>
     <row r="207">
-      <c t="s" s="2" r="A207">
+      <c t="s" s="1" r="A207">
         <v>3181</v>
       </c>
       <c t="s" s="3" r="B207">
@@ -25656,7 +25656,7 @@
       </c>
     </row>
     <row r="208">
-      <c t="s" s="2" r="A208">
+      <c t="s" s="1" r="A208">
         <v>3197</v>
       </c>
       <c t="s" s="3" r="B208">
@@ -25731,7 +25731,7 @@
       </c>
     </row>
     <row r="209">
-      <c t="s" s="2" r="A209">
+      <c t="s" s="1" r="A209">
         <v>3221</v>
       </c>
       <c t="s" s="3" r="B209">
@@ -25806,7 +25806,7 @@
       </c>
     </row>
     <row r="210">
-      <c t="s" s="2" r="A210">
+      <c t="s" s="1" r="A210">
         <v>3245</v>
       </c>
       <c t="s" s="3" r="B210">
@@ -25881,7 +25881,7 @@
       </c>
     </row>
     <row r="211">
-      <c t="s" s="2" r="A211">
+      <c t="s" s="1" r="A211">
         <v>3266</v>
       </c>
       <c t="s" s="3" r="B211">
@@ -25956,7 +25956,7 @@
       </c>
     </row>
     <row r="212">
-      <c t="s" s="2" r="A212">
+      <c t="s" s="1" r="A212">
         <v>3290</v>
       </c>
       <c t="s" s="3" r="B212">
@@ -26031,7 +26031,7 @@
       </c>
     </row>
     <row r="213">
-      <c t="s" s="2" r="A213">
+      <c t="s" s="1" r="A213">
         <v>3312</v>
       </c>
       <c t="s" s="3" r="B213">
@@ -26106,7 +26106,7 @@
       </c>
     </row>
     <row r="214">
-      <c t="s" s="2" r="A214">
+      <c t="s" s="1" r="A214">
         <v>3336</v>
       </c>
       <c t="s" s="3" r="B214">
@@ -26181,7 +26181,7 @@
       </c>
     </row>
     <row r="215">
-      <c t="s" s="2" r="A215">
+      <c t="s" s="1" r="A215">
         <v>3357</v>
       </c>
       <c t="s" s="3" r="B215">
@@ -26256,7 +26256,7 @@
       </c>
     </row>
     <row r="216">
-      <c t="s" s="2" r="A216">
+      <c t="s" s="1" r="A216">
         <v>3380</v>
       </c>
       <c t="s" s="3" r="B216">
@@ -26331,7 +26331,7 @@
       </c>
     </row>
     <row r="217">
-      <c t="s" s="2" r="A217">
+      <c t="s" s="1" r="A217">
         <v>3404</v>
       </c>
       <c t="s" s="3" r="B217">
@@ -26406,7 +26406,7 @@
       </c>
     </row>
     <row r="218">
-      <c t="s" s="2" r="A218">
+      <c t="s" s="1" r="A218">
         <v>3427</v>
       </c>
       <c t="s" s="3" r="B218">
@@ -26481,7 +26481,7 @@
       </c>
     </row>
     <row r="219">
-      <c t="s" s="2" r="A219">
+      <c t="s" s="1" r="A219">
         <v>3451</v>
       </c>
       <c t="s" s="3" r="B219">
@@ -26556,7 +26556,7 @@
       </c>
     </row>
     <row r="220">
-      <c t="s" s="2" r="A220">
+      <c t="s" s="1" r="A220">
         <v>3474</v>
       </c>
       <c t="s" s="3" r="B220">
@@ -26631,7 +26631,7 @@
       </c>
     </row>
     <row r="221">
-      <c t="s" s="2" r="A221">
+      <c t="s" s="1" r="A221">
         <v>3497</v>
       </c>
       <c t="s" s="3" r="B221">
@@ -26706,7 +26706,7 @@
       </c>
     </row>
     <row r="222">
-      <c t="s" s="2" r="A222">
+      <c t="s" s="1" r="A222">
         <v>3520</v>
       </c>
       <c t="s" s="3" r="B222">
@@ -26781,7 +26781,7 @@
       </c>
     </row>
     <row r="223">
-      <c t="s" s="2" r="A223">
+      <c t="s" s="1" r="A223">
         <v>3544</v>
       </c>
       <c t="s" s="3" r="B223">
@@ -26856,7 +26856,7 @@
       </c>
     </row>
     <row r="224">
-      <c t="s" s="2" r="A224">
+      <c t="s" s="1" r="A224">
         <v>3568</v>
       </c>
       <c t="s" s="3" r="B224">
@@ -26933,7 +26933,7 @@
       </c>
     </row>
     <row r="225">
-      <c t="s" s="2" r="A225">
+      <c t="s" s="1" r="A225">
         <v>3586</v>
       </c>
       <c t="s" s="3" r="B225">
@@ -27008,7 +27008,7 @@
       </c>
     </row>
     <row r="226">
-      <c t="s" s="2" r="A226">
+      <c t="s" s="1" r="A226">
         <v>3599</v>
       </c>
       <c t="s" s="3" r="B226">
@@ -27083,7 +27083,7 @@
       </c>
     </row>
     <row r="227">
-      <c t="s" s="2" r="A227">
+      <c t="s" s="1" r="A227">
         <v>3603</v>
       </c>
       <c t="s" s="3" r="B227">
@@ -27158,7 +27158,7 @@
       </c>
     </row>
     <row r="228">
-      <c t="s" s="2" r="A228">
+      <c t="s" s="1" r="A228">
         <v>3609</v>
       </c>
       <c t="s" s="3" r="B228">
@@ -27233,7 +27233,7 @@
       </c>
     </row>
     <row r="229">
-      <c t="s" s="2" r="A229">
+      <c t="s" s="1" r="A229">
         <v>3622</v>
       </c>
       <c t="s" s="3" r="B229">
@@ -27308,7 +27308,7 @@
       </c>
     </row>
     <row r="230">
-      <c t="s" s="2" r="A230">
+      <c t="s" s="1" r="A230">
         <v>3633</v>
       </c>
       <c t="s" s="3" r="B230">
@@ -27383,7 +27383,7 @@
       </c>
     </row>
     <row r="231">
-      <c t="s" s="2" r="A231">
+      <c t="s" s="1" r="A231">
         <v>3650</v>
       </c>
       <c t="s" s="3" r="B231">
@@ -27458,7 +27458,7 @@
       </c>
     </row>
     <row r="232">
-      <c t="s" s="2" r="A232">
+      <c t="s" s="1" r="A232">
         <v>3667</v>
       </c>
       <c t="s" s="3" r="B232">
@@ -27535,7 +27535,7 @@
       </c>
     </row>
     <row customHeight="1" r="233" ht="26.25">
-      <c t="s" s="2" r="A233">
+      <c t="s" s="1" r="A233">
         <v>3689</v>
       </c>
       <c t="s" s="3" r="B233">
@@ -27610,7 +27610,7 @@
       </c>
     </row>
     <row r="234">
-      <c s="2" r="A234"/>
+      <c s="1" r="A234"/>
       <c s="3" r="B234"/>
       <c s="3" r="C234"/>
       <c s="3" r="D234"/>
@@ -27637,7 +27637,7 @@
       <c s="3" r="Y234"/>
     </row>
     <row r="235">
-      <c s="2" r="A235"/>
+      <c s="1" r="A235"/>
       <c s="3" r="B235"/>
       <c s="3" r="C235"/>
       <c s="3" r="D235"/>

</xml_diff>

<commit_message>
Using YouTube's WATCHED element instead. Fixed another minor bug.
</commit_message>
<xml_diff>
--- a/Translation.xlsx
+++ b/Translation.xlsx
@@ -675,7 +675,7 @@
     <t>SETTINGS_WATCHED</t>
   </si>
   <si>
-    <t>Watched</t>
+    <t>WATCHED</t>
   </si>
   <si>
     <t>İzlendi</t>
@@ -15645,6 +15645,9 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="49" borderId="0" fontId="0" applyNumberFormat="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="10" borderId="0" fontId="0" applyNumberFormat="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
@@ -15656,9 +15659,6 @@
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="10" borderId="0" applyFont="1" fontId="3" applyNumberFormat="1">
       <alignment vertical="bottom" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="49" borderId="0" fontId="0" applyNumberFormat="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="49" borderId="0" fontId="0" applyNumberFormat="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
@@ -15761,11 +15761,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="534046727"/>
-        <c:axId val="1082000161"/>
+        <c:axId val="256132799"/>
+        <c:axId val="1738940585"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="534046727"/>
+        <c:axId val="256132799"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15800,10 +15800,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1082000161"/>
+        <c:crossAx val="1738940585"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1082000161"/>
+        <c:axId val="1738940585"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15842,7 +15842,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="534046727"/>
+        <c:crossAx val="256132799"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
@@ -15914,85 +15914,85 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c s="2" r="A1"/>
-      <c t="s" s="2" r="B1">
+      <c s="3" r="A1"/>
+      <c t="s" s="3" r="B1">
         <v>0</v>
       </c>
-      <c t="s" s="2" r="C1">
+      <c t="s" s="3" r="C1">
         <v>1</v>
       </c>
-      <c t="s" s="2" r="D1">
+      <c t="s" s="3" r="D1">
         <v>2</v>
       </c>
-      <c t="s" s="2" r="E1">
+      <c t="s" s="3" r="E1">
         <v>3</v>
       </c>
-      <c t="s" s="2" r="F1">
+      <c t="s" s="3" r="F1">
         <v>4</v>
       </c>
-      <c t="s" s="2" r="G1">
+      <c t="s" s="3" r="G1">
         <v>5</v>
       </c>
-      <c t="s" s="2" r="H1">
+      <c t="s" s="3" r="H1">
         <v>6</v>
       </c>
-      <c t="s" s="2" r="I1">
+      <c t="s" s="3" r="I1">
         <v>7</v>
       </c>
-      <c t="s" s="2" r="J1">
+      <c t="s" s="3" r="J1">
         <v>8</v>
       </c>
-      <c t="s" s="2" r="K1">
+      <c t="s" s="3" r="K1">
         <v>9</v>
       </c>
-      <c t="s" s="2" r="L1">
+      <c t="s" s="3" r="L1">
         <v>10</v>
       </c>
-      <c t="s" s="2" r="M1">
+      <c t="s" s="3" r="M1">
         <v>11</v>
       </c>
-      <c t="s" s="2" r="N1">
+      <c t="s" s="3" r="N1">
         <v>12</v>
       </c>
-      <c t="s" s="2" r="O1">
+      <c t="s" s="3" r="O1">
         <v>13</v>
       </c>
-      <c t="s" s="2" r="P1">
+      <c t="s" s="3" r="P1">
         <v>14</v>
       </c>
-      <c t="s" s="2" r="Q1">
+      <c t="s" s="3" r="Q1">
         <v>15</v>
       </c>
-      <c t="s" s="2" r="R1">
+      <c t="s" s="3" r="R1">
         <v>16</v>
       </c>
-      <c t="s" s="2" r="S1">
+      <c t="s" s="3" r="S1">
         <v>17</v>
       </c>
-      <c t="s" s="2" r="T1">
+      <c t="s" s="3" r="T1">
         <v>18</v>
       </c>
-      <c t="s" s="2" r="U1">
+      <c t="s" s="3" r="U1">
         <v>19</v>
       </c>
-      <c t="s" s="2" r="V1">
+      <c t="s" s="3" r="V1">
         <v>20</v>
       </c>
-      <c t="s" s="2" r="W1">
+      <c t="s" s="3" r="W1">
         <v>21</v>
       </c>
-      <c t="s" s="2" r="X1">
+      <c t="s" s="3" r="X1">
         <v>22</v>
       </c>
-      <c t="s" s="2" r="Y1">
+      <c t="s" s="3" r="Y1">
         <v>23</v>
       </c>
-      <c t="s" s="2" r="Z1">
+      <c t="s" s="3" r="Z1">
         <v>24</v>
       </c>
     </row>
     <row r="2">
-      <c t="s" s="2" r="A2">
+      <c t="s" s="3" r="A2">
         <v>25</v>
       </c>
       <c t="s" s="6" r="B2">
@@ -16072,7 +16072,7 @@
       </c>
     </row>
     <row r="3">
-      <c t="s" s="2" r="A3">
+      <c t="s" s="3" r="A3">
         <v>51</v>
       </c>
       <c t="s" s="6" r="B3">
@@ -16152,7 +16152,7 @@
       </c>
     </row>
     <row r="4">
-      <c t="s" s="2" r="A4">
+      <c t="s" s="3" r="A4">
         <v>76</v>
       </c>
       <c t="s" s="6" r="B4">
@@ -16232,7 +16232,7 @@
       </c>
     </row>
     <row r="5">
-      <c t="s" s="2" r="A5">
+      <c t="s" s="3" r="A5">
         <v>77</v>
       </c>
       <c t="s" s="6" r="B5">
@@ -16312,7 +16312,7 @@
       </c>
     </row>
     <row r="6">
-      <c t="s" s="2" r="A6">
+      <c t="s" s="3" r="A6">
         <v>103</v>
       </c>
       <c t="s" s="6" r="B6">
@@ -16352,7 +16352,7 @@
       <c s="6" r="Z6"/>
     </row>
     <row r="7">
-      <c t="s" s="2" r="A7">
+      <c t="s" s="3" r="A7">
         <v>109</v>
       </c>
       <c t="s" s="6" r="B7">
@@ -16392,7 +16392,7 @@
       <c s="6" r="Z7"/>
     </row>
     <row r="8">
-      <c t="s" s="2" r="A8">
+      <c t="s" s="3" r="A8">
         <v>112</v>
       </c>
       <c t="s" s="6" r="B8">
@@ -16434,7 +16434,7 @@
       <c s="6" r="Z8"/>
     </row>
     <row r="9">
-      <c t="s" s="2" r="A9">
+      <c t="s" s="3" r="A9">
         <v>119</v>
       </c>
       <c t="s" s="6" r="B9">
@@ -16474,7 +16474,7 @@
       <c s="6" r="Z9"/>
     </row>
     <row r="10">
-      <c t="s" s="2" r="A10">
+      <c t="s" s="3" r="A10">
         <v>125</v>
       </c>
       <c t="s" s="6" r="B10">
@@ -16516,7 +16516,7 @@
       <c s="6" r="Z10"/>
     </row>
     <row r="11">
-      <c t="s" s="2" r="A11">
+      <c t="s" s="3" r="A11">
         <v>132</v>
       </c>
       <c t="s" s="6" r="B11">
@@ -16558,7 +16558,7 @@
       <c s="6" r="Z11"/>
     </row>
     <row r="12">
-      <c t="s" s="2" r="A12">
+      <c t="s" s="3" r="A12">
         <v>134</v>
       </c>
       <c t="s" s="6" r="B12">
@@ -16608,7 +16608,7 @@
       </c>
     </row>
     <row r="13">
-      <c t="s" s="2" r="A13">
+      <c t="s" s="3" r="A13">
         <v>145</v>
       </c>
       <c t="s" s="6" r="B13">
@@ -16658,7 +16658,7 @@
       </c>
     </row>
     <row r="14">
-      <c t="s" s="2" r="A14">
+      <c t="s" s="3" r="A14">
         <v>156</v>
       </c>
       <c t="s" s="6" r="B14">
@@ -16706,7 +16706,7 @@
       </c>
     </row>
     <row r="15">
-      <c t="s" s="2" r="A15">
+      <c t="s" s="3" r="A15">
         <v>166</v>
       </c>
       <c t="s" s="6" r="B15">
@@ -16760,7 +16760,7 @@
       </c>
     </row>
     <row r="16">
-      <c t="s" s="2" r="A16">
+      <c t="s" s="3" r="A16">
         <v>179</v>
       </c>
       <c t="s" s="6" r="B16">
@@ -16814,7 +16814,7 @@
       </c>
     </row>
     <row r="17">
-      <c t="s" s="2" r="A17">
+      <c t="s" s="3" r="A17">
         <v>192</v>
       </c>
       <c t="s" s="6" r="B17">
@@ -16868,7 +16868,7 @@
       </c>
     </row>
     <row r="18">
-      <c t="s" s="2" r="A18">
+      <c t="s" s="3" r="A18">
         <v>205</v>
       </c>
       <c t="s" s="6" r="B18">
@@ -16922,7 +16922,7 @@
       </c>
     </row>
     <row r="19">
-      <c t="s" s="2" r="A19">
+      <c t="s" s="3" r="A19">
         <v>218</v>
       </c>
       <c t="s" s="6" r="B19">
@@ -16976,7 +16976,7 @@
       </c>
     </row>
     <row r="20">
-      <c t="s" s="2" r="A20">
+      <c t="s" s="3" r="A20">
         <v>231</v>
       </c>
       <c t="s" s="6" r="B20">
@@ -17030,7 +17030,7 @@
       </c>
     </row>
     <row r="21">
-      <c t="s" s="2" r="A21">
+      <c t="s" s="3" r="A21">
         <v>244</v>
       </c>
       <c t="s" s="6" r="B21">
@@ -17084,7 +17084,7 @@
       </c>
     </row>
     <row r="22">
-      <c t="s" s="2" r="A22">
+      <c t="s" s="3" r="A22">
         <v>257</v>
       </c>
       <c t="s" s="6" r="B22">
@@ -17138,7 +17138,7 @@
       </c>
     </row>
     <row r="23">
-      <c t="s" s="2" r="A23">
+      <c t="s" s="3" r="A23">
         <v>270</v>
       </c>
       <c t="s" s="6" r="B23">
@@ -17194,7 +17194,7 @@
       </c>
     </row>
     <row r="24">
-      <c t="s" s="2" r="A24">
+      <c t="s" s="3" r="A24">
         <v>284</v>
       </c>
       <c t="s" s="6" r="B24">
@@ -17250,7 +17250,7 @@
       </c>
     </row>
     <row r="25">
-      <c t="s" s="2" r="A25">
+      <c t="s" s="3" r="A25">
         <v>298</v>
       </c>
       <c t="s" s="6" r="B25">
@@ -17304,7 +17304,7 @@
       </c>
     </row>
     <row r="26">
-      <c t="s" s="2" r="A26">
+      <c t="s" s="3" r="A26">
         <v>311</v>
       </c>
       <c t="s" s="6" r="B26">
@@ -17360,7 +17360,7 @@
       </c>
     </row>
     <row r="27">
-      <c t="s" s="2" r="A27">
+      <c t="s" s="3" r="A27">
         <v>325</v>
       </c>
       <c t="s" s="6" r="B27">
@@ -17416,7 +17416,7 @@
       </c>
     </row>
     <row r="28">
-      <c t="s" s="2" r="A28">
+      <c t="s" s="3" r="A28">
         <v>339</v>
       </c>
       <c t="s" s="6" r="B28">
@@ -17472,7 +17472,7 @@
       </c>
     </row>
     <row r="29">
-      <c t="s" s="2" r="A29">
+      <c t="s" s="3" r="A29">
         <v>353</v>
       </c>
       <c t="s" s="6" r="B29">
@@ -17528,7 +17528,7 @@
       </c>
     </row>
     <row r="30">
-      <c t="s" s="2" r="A30">
+      <c t="s" s="3" r="A30">
         <v>367</v>
       </c>
       <c t="s" s="6" r="B30">
@@ -17584,7 +17584,7 @@
       </c>
     </row>
     <row r="31">
-      <c t="s" s="2" r="A31">
+      <c t="s" s="3" r="A31">
         <v>381</v>
       </c>
       <c t="s" s="6" r="B31">
@@ -17640,16 +17640,16 @@
       </c>
     </row>
     <row r="32">
-      <c t="s" s="2" r="A32">
+      <c t="s" s="3" r="A32">
         <v>395</v>
       </c>
-      <c t="s" s="5" r="B32">
+      <c t="s" s="1" r="B32">
         <v>396</v>
       </c>
       <c t="s" s="6" r="C32">
         <v>396</v>
       </c>
-      <c t="s" s="5" r="D32">
+      <c t="s" s="1" r="D32">
         <v>396</v>
       </c>
       <c s="6" r="E32"/>
@@ -17657,42 +17657,42 @@
         <v>396</v>
       </c>
       <c s="6" r="G32"/>
-      <c t="s" s="5" r="H32">
+      <c t="s" s="1" r="H32">
         <v>396</v>
       </c>
       <c s="6" r="I32"/>
       <c s="6" r="J32"/>
       <c s="6" r="K32"/>
       <c s="6" r="L32"/>
-      <c t="s" s="5" r="M32">
+      <c t="s" s="1" r="M32">
         <v>396</v>
       </c>
-      <c t="s" s="5" r="N32">
+      <c t="s" s="1" r="N32">
         <v>396</v>
       </c>
       <c s="6" r="O32"/>
       <c s="6" r="P32"/>
-      <c t="s" s="5" r="Q32">
+      <c t="s" s="1" r="Q32">
         <v>396</v>
       </c>
       <c s="6" r="R32"/>
       <c s="6" r="S32"/>
-      <c t="s" s="5" r="T32">
+      <c t="s" s="1" r="T32">
         <v>396</v>
       </c>
-      <c t="s" s="5" r="U32">
+      <c t="s" s="1" r="U32">
         <v>396</v>
       </c>
       <c s="6" r="V32"/>
       <c s="6" r="W32"/>
       <c s="6" r="X32"/>
       <c s="6" r="Y32"/>
-      <c t="s" s="5" r="Z32">
+      <c t="s" s="1" r="Z32">
         <v>396</v>
       </c>
     </row>
     <row r="33">
-      <c t="s" s="2" r="A33">
+      <c t="s" s="3" r="A33">
         <v>397</v>
       </c>
       <c t="s" s="6" r="B33">
@@ -17748,7 +17748,7 @@
       </c>
     </row>
     <row r="34">
-      <c t="s" s="2" r="A34">
+      <c t="s" s="3" r="A34">
         <v>411</v>
       </c>
       <c t="s" s="6" r="B34">
@@ -17804,7 +17804,7 @@
       </c>
     </row>
     <row r="35">
-      <c t="s" s="2" r="A35">
+      <c t="s" s="3" r="A35">
         <v>425</v>
       </c>
       <c t="s" s="6" r="B35">
@@ -17860,7 +17860,7 @@
       </c>
     </row>
     <row r="36">
-      <c t="s" s="2" r="A36">
+      <c t="s" s="3" r="A36">
         <v>439</v>
       </c>
       <c t="s" s="6" r="B36">
@@ -17916,7 +17916,7 @@
       </c>
     </row>
     <row r="37">
-      <c t="s" s="2" r="A37">
+      <c t="s" s="3" r="A37">
         <v>453</v>
       </c>
       <c t="s" s="6" r="B37">
@@ -17972,7 +17972,7 @@
       </c>
     </row>
     <row r="38">
-      <c t="s" s="2" r="A38">
+      <c t="s" s="3" r="A38">
         <v>467</v>
       </c>
       <c t="s" s="6" r="B38">
@@ -18024,7 +18024,7 @@
       </c>
     </row>
     <row r="39">
-      <c t="s" s="2" r="A39">
+      <c t="s" s="3" r="A39">
         <v>477</v>
       </c>
       <c t="s" s="6" r="B39">
@@ -18078,7 +18078,7 @@
       </c>
     </row>
     <row r="40">
-      <c t="s" s="2" r="A40">
+      <c t="s" s="3" r="A40">
         <v>490</v>
       </c>
       <c t="s" s="6" r="B40">
@@ -18134,7 +18134,7 @@
       </c>
     </row>
     <row r="41">
-      <c t="s" s="2" r="A41">
+      <c t="s" s="3" r="A41">
         <v>504</v>
       </c>
       <c t="s" s="6" r="B41">
@@ -18190,7 +18190,7 @@
       </c>
     </row>
     <row r="42">
-      <c t="s" s="2" r="A42">
+      <c t="s" s="3" r="A42">
         <v>518</v>
       </c>
       <c t="s" s="6" r="B42">
@@ -18246,7 +18246,7 @@
       </c>
     </row>
     <row r="43">
-      <c t="s" s="2" r="A43">
+      <c t="s" s="3" r="A43">
         <v>532</v>
       </c>
       <c t="s" s="6" r="B43">
@@ -18302,7 +18302,7 @@
       </c>
     </row>
     <row r="44">
-      <c t="s" s="2" r="A44">
+      <c t="s" s="3" r="A44">
         <v>546</v>
       </c>
       <c t="s" s="6" r="B44">
@@ -18354,7 +18354,7 @@
       </c>
     </row>
     <row r="45">
-      <c t="s" s="2" r="A45">
+      <c t="s" s="3" r="A45">
         <v>558</v>
       </c>
       <c t="s" s="6" r="B45">
@@ -18408,7 +18408,7 @@
       </c>
     </row>
     <row r="46">
-      <c t="s" s="2" r="A46">
+      <c t="s" s="3" r="A46">
         <v>571</v>
       </c>
       <c t="s" s="6" r="B46">
@@ -18462,7 +18462,7 @@
       </c>
     </row>
     <row r="47">
-      <c t="s" s="2" r="A47">
+      <c t="s" s="3" r="A47">
         <v>584</v>
       </c>
       <c t="s" s="6" r="B47">
@@ -18518,7 +18518,7 @@
       </c>
     </row>
     <row r="48">
-      <c t="s" s="2" r="A48">
+      <c t="s" s="3" r="A48">
         <v>598</v>
       </c>
       <c t="s" s="6" r="B48">
@@ -18574,7 +18574,7 @@
       </c>
     </row>
     <row r="49">
-      <c t="s" s="2" r="A49">
+      <c t="s" s="3" r="A49">
         <v>601</v>
       </c>
       <c t="s" s="6" r="B49">
@@ -18628,7 +18628,7 @@
       </c>
     </row>
     <row r="50">
-      <c t="s" s="2" r="A50">
+      <c t="s" s="3" r="A50">
         <v>614</v>
       </c>
       <c t="s" s="6" r="B50">
@@ -18684,7 +18684,7 @@
       </c>
     </row>
     <row r="51">
-      <c t="s" s="2" r="A51">
+      <c t="s" s="3" r="A51">
         <v>628</v>
       </c>
       <c t="s" s="6" r="B51">
@@ -18738,7 +18738,7 @@
       </c>
     </row>
     <row r="52">
-      <c t="s" s="2" r="A52">
+      <c t="s" s="3" r="A52">
         <v>641</v>
       </c>
       <c t="s" s="6" r="B52">
@@ -18794,7 +18794,7 @@
       </c>
     </row>
     <row r="53">
-      <c t="s" s="2" r="A53">
+      <c t="s" s="3" r="A53">
         <v>655</v>
       </c>
       <c t="s" s="6" r="B53">
@@ -18850,7 +18850,7 @@
       </c>
     </row>
     <row r="54">
-      <c t="s" s="2" r="A54">
+      <c t="s" s="3" r="A54">
         <v>669</v>
       </c>
       <c t="s" s="6" r="B54">
@@ -18908,7 +18908,7 @@
       </c>
     </row>
     <row r="55">
-      <c t="s" s="2" r="A55">
+      <c t="s" s="3" r="A55">
         <v>684</v>
       </c>
       <c t="s" s="6" r="B55">
@@ -18966,7 +18966,7 @@
       </c>
     </row>
     <row r="56">
-      <c t="s" s="2" r="A56">
+      <c t="s" s="3" r="A56">
         <v>696</v>
       </c>
       <c t="s" s="6" r="B56">
@@ -19022,7 +19022,7 @@
       </c>
     </row>
     <row r="57">
-      <c t="s" s="2" r="A57">
+      <c t="s" s="3" r="A57">
         <v>710</v>
       </c>
       <c t="s" s="6" r="B57">
@@ -19078,7 +19078,7 @@
       </c>
     </row>
     <row r="58">
-      <c t="s" s="2" r="A58">
+      <c t="s" s="3" r="A58">
         <v>724</v>
       </c>
       <c t="s" s="6" r="B58">
@@ -19134,7 +19134,7 @@
       </c>
     </row>
     <row r="59">
-      <c t="s" s="2" r="A59">
+      <c t="s" s="3" r="A59">
         <v>738</v>
       </c>
       <c t="s" s="6" r="B59">
@@ -19190,7 +19190,7 @@
       </c>
     </row>
     <row r="60">
-      <c t="s" s="2" r="A60">
+      <c t="s" s="3" r="A60">
         <v>752</v>
       </c>
       <c t="s" s="6" r="B60">
@@ -19246,7 +19246,7 @@
       </c>
     </row>
     <row r="61">
-      <c t="s" s="2" r="A61">
+      <c t="s" s="3" r="A61">
         <v>765</v>
       </c>
       <c t="s" s="6" r="B61">
@@ -19302,7 +19302,7 @@
       </c>
     </row>
     <row r="62">
-      <c t="s" s="2" r="A62">
+      <c t="s" s="3" r="A62">
         <v>779</v>
       </c>
       <c t="s" s="6" r="B62">
@@ -19358,7 +19358,7 @@
       </c>
     </row>
     <row r="63">
-      <c t="s" s="2" r="A63">
+      <c t="s" s="3" r="A63">
         <v>793</v>
       </c>
       <c t="s" s="6" r="B63">
@@ -19414,7 +19414,7 @@
       </c>
     </row>
     <row r="64">
-      <c t="s" s="2" r="A64">
+      <c t="s" s="3" r="A64">
         <v>807</v>
       </c>
       <c t="s" s="6" r="B64">
@@ -19472,7 +19472,7 @@
       </c>
     </row>
     <row r="65">
-      <c t="s" s="2" r="A65">
+      <c t="s" s="3" r="A65">
         <v>821</v>
       </c>
       <c t="s" s="6" r="B65">
@@ -19528,7 +19528,7 @@
       </c>
     </row>
     <row r="66">
-      <c t="s" s="2" r="A66">
+      <c t="s" s="3" r="A66">
         <v>835</v>
       </c>
       <c t="s" s="6" r="B66">
@@ -19586,7 +19586,7 @@
       </c>
     </row>
     <row r="67">
-      <c t="s" s="2" r="A67">
+      <c t="s" s="3" r="A67">
         <v>850</v>
       </c>
       <c t="s" s="6" r="B67">
@@ -19644,7 +19644,7 @@
       </c>
     </row>
     <row r="68">
-      <c t="s" s="2" r="A68">
+      <c t="s" s="3" r="A68">
         <v>865</v>
       </c>
       <c t="s" s="6" r="B68">
@@ -19698,7 +19698,7 @@
       </c>
     </row>
     <row r="69">
-      <c t="s" s="2" r="A69">
+      <c t="s" s="3" r="A69">
         <v>877</v>
       </c>
       <c t="s" s="6" r="B69">
@@ -19756,7 +19756,7 @@
       </c>
     </row>
     <row r="70">
-      <c t="s" s="2" r="A70">
+      <c t="s" s="3" r="A70">
         <v>891</v>
       </c>
       <c t="s" s="6" r="B70">
@@ -19812,7 +19812,7 @@
       </c>
     </row>
     <row r="71">
-      <c t="s" s="2" r="A71">
+      <c t="s" s="3" r="A71">
         <v>905</v>
       </c>
       <c t="s" s="6" r="B71">
@@ -19868,7 +19868,7 @@
       </c>
     </row>
     <row r="72">
-      <c t="s" s="2" r="A72">
+      <c t="s" s="3" r="A72">
         <v>919</v>
       </c>
       <c t="s" s="6" r="B72">
@@ -19924,7 +19924,7 @@
       </c>
     </row>
     <row r="73">
-      <c t="s" s="2" r="A73">
+      <c t="s" s="3" r="A73">
         <v>933</v>
       </c>
       <c t="s" s="6" r="B73">
@@ -19982,7 +19982,7 @@
       </c>
     </row>
     <row r="74">
-      <c t="s" s="2" r="A74">
+      <c t="s" s="3" r="A74">
         <v>947</v>
       </c>
       <c t="s" s="6" r="B74">
@@ -20040,7 +20040,7 @@
       </c>
     </row>
     <row r="75">
-      <c t="s" s="2" r="A75">
+      <c t="s" s="3" r="A75">
         <v>961</v>
       </c>
       <c t="s" s="6" r="B75">
@@ -20098,7 +20098,7 @@
       </c>
     </row>
     <row r="76">
-      <c t="s" s="2" r="A76">
+      <c t="s" s="3" r="A76">
         <v>976</v>
       </c>
       <c t="s" s="6" r="B76">
@@ -20154,7 +20154,7 @@
       </c>
     </row>
     <row r="77">
-      <c t="s" s="2" r="A77">
+      <c t="s" s="3" r="A77">
         <v>990</v>
       </c>
       <c t="s" s="6" r="B77">
@@ -20212,7 +20212,7 @@
       </c>
     </row>
     <row r="78">
-      <c t="s" s="2" r="A78">
+      <c t="s" s="3" r="A78">
         <v>1005</v>
       </c>
       <c t="s" s="6" r="B78">
@@ -20270,7 +20270,7 @@
       </c>
     </row>
     <row r="79">
-      <c t="s" s="2" r="A79">
+      <c t="s" s="3" r="A79">
         <v>1020</v>
       </c>
       <c t="s" s="6" r="B79">
@@ -20328,7 +20328,7 @@
       </c>
     </row>
     <row r="80">
-      <c t="s" s="2" r="A80">
+      <c t="s" s="3" r="A80">
         <v>1035</v>
       </c>
       <c t="s" s="6" r="B80">
@@ -20384,7 +20384,7 @@
       </c>
     </row>
     <row r="81">
-      <c t="s" s="2" r="A81">
+      <c t="s" s="3" r="A81">
         <v>1049</v>
       </c>
       <c t="s" s="6" r="B81">
@@ -20440,7 +20440,7 @@
       </c>
     </row>
     <row r="82">
-      <c t="s" s="2" r="A82">
+      <c t="s" s="3" r="A82">
         <v>1063</v>
       </c>
       <c t="s" s="6" r="B82">
@@ -20496,7 +20496,7 @@
       </c>
     </row>
     <row r="83">
-      <c t="s" s="2" r="A83">
+      <c t="s" s="3" r="A83">
         <v>1077</v>
       </c>
       <c t="s" s="6" r="B83">
@@ -20552,7 +20552,7 @@
       </c>
     </row>
     <row r="84">
-      <c t="s" s="2" r="A84">
+      <c t="s" s="3" r="A84">
         <v>1091</v>
       </c>
       <c t="s" s="6" r="B84">
@@ -20608,7 +20608,7 @@
       </c>
     </row>
     <row r="85">
-      <c t="s" s="2" r="A85">
+      <c t="s" s="3" r="A85">
         <v>1105</v>
       </c>
       <c t="s" s="6" r="B85">
@@ -20666,7 +20666,7 @@
       </c>
     </row>
     <row r="86">
-      <c t="s" s="2" r="A86">
+      <c t="s" s="3" r="A86">
         <v>1109</v>
       </c>
       <c t="s" s="6" r="B86">
@@ -20722,7 +20722,7 @@
       </c>
     </row>
     <row r="87">
-      <c t="s" s="2" r="A87">
+      <c t="s" s="3" r="A87">
         <v>1121</v>
       </c>
       <c t="s" s="6" r="B87">
@@ -20778,7 +20778,7 @@
       </c>
     </row>
     <row r="88">
-      <c t="s" s="2" r="A88">
+      <c t="s" s="3" r="A88">
         <v>1135</v>
       </c>
       <c t="s" s="6" r="B88">
@@ -20836,7 +20836,7 @@
       </c>
     </row>
     <row r="89">
-      <c t="s" s="2" r="A89">
+      <c t="s" s="3" r="A89">
         <v>1150</v>
       </c>
       <c t="s" s="6" r="B89">
@@ -20884,7 +20884,7 @@
       </c>
     </row>
     <row r="90">
-      <c t="s" s="2" r="A90">
+      <c t="s" s="3" r="A90">
         <v>1159</v>
       </c>
       <c t="s" s="6" r="B90">
@@ -20942,7 +20942,7 @@
       </c>
     </row>
     <row r="91">
-      <c t="s" s="2" r="A91">
+      <c t="s" s="3" r="A91">
         <v>1174</v>
       </c>
       <c t="s" s="6" r="B91">
@@ -21002,7 +21002,7 @@
       </c>
     </row>
     <row r="92">
-      <c t="s" s="2" r="A92">
+      <c t="s" s="3" r="A92">
         <v>1190</v>
       </c>
       <c t="s" s="6" r="B92">
@@ -21060,7 +21060,7 @@
       </c>
     </row>
     <row r="93">
-      <c t="s" s="2" r="A93">
+      <c t="s" s="3" r="A93">
         <v>1205</v>
       </c>
       <c t="s" s="6" r="B93">
@@ -21118,7 +21118,7 @@
       </c>
     </row>
     <row r="94">
-      <c t="s" s="2" r="A94">
+      <c t="s" s="3" r="A94">
         <v>1218</v>
       </c>
       <c t="s" s="6" r="B94">
@@ -21176,7 +21176,7 @@
       </c>
     </row>
     <row r="95">
-      <c t="s" s="2" r="A95">
+      <c t="s" s="3" r="A95">
         <v>1233</v>
       </c>
       <c t="s" s="6" r="B95">
@@ -21234,7 +21234,7 @@
       </c>
     </row>
     <row r="96">
-      <c t="s" s="2" r="A96">
+      <c t="s" s="3" r="A96">
         <v>1246</v>
       </c>
       <c t="s" s="6" r="B96">
@@ -21292,7 +21292,7 @@
       </c>
     </row>
     <row r="97">
-      <c t="s" s="2" r="A97">
+      <c t="s" s="3" r="A97">
         <v>1260</v>
       </c>
       <c t="s" s="6" r="B97">
@@ -21350,7 +21350,7 @@
       </c>
     </row>
     <row r="98">
-      <c t="s" s="2" r="A98">
+      <c t="s" s="3" r="A98">
         <v>1275</v>
       </c>
       <c t="s" s="6" r="B98">
@@ -21406,7 +21406,7 @@
       </c>
     </row>
     <row r="99">
-      <c t="s" s="2" r="A99">
+      <c t="s" s="3" r="A99">
         <v>1288</v>
       </c>
       <c t="s" s="6" r="B99">
@@ -21462,7 +21462,7 @@
       </c>
     </row>
     <row r="100">
-      <c t="s" s="2" r="A100">
+      <c t="s" s="3" r="A100">
         <v>1302</v>
       </c>
       <c t="s" s="6" r="B100">
@@ -21520,7 +21520,7 @@
       </c>
     </row>
     <row r="101">
-      <c t="s" s="2" r="A101">
+      <c t="s" s="3" r="A101">
         <v>1317</v>
       </c>
       <c t="s" s="6" r="B101">
@@ -21578,7 +21578,7 @@
       </c>
     </row>
     <row r="102">
-      <c t="s" s="2" r="A102">
+      <c t="s" s="3" r="A102">
         <v>1332</v>
       </c>
       <c t="s" s="6" r="B102">
@@ -21636,7 +21636,7 @@
       </c>
     </row>
     <row r="103">
-      <c t="s" s="2" r="A103">
+      <c t="s" s="3" r="A103">
         <v>1334</v>
       </c>
       <c t="s" s="6" r="B103">
@@ -21702,7 +21702,7 @@
       </c>
     </row>
     <row r="104">
-      <c t="s" s="2" r="A104">
+      <c t="s" s="3" r="A104">
         <v>1353</v>
       </c>
       <c t="s" s="6" r="B104">
@@ -21770,7 +21770,7 @@
       </c>
     </row>
     <row r="105">
-      <c t="s" s="2" r="A105">
+      <c t="s" s="3" r="A105">
         <v>1373</v>
       </c>
       <c t="s" s="6" r="B105">
@@ -21838,7 +21838,7 @@
       </c>
     </row>
     <row r="106">
-      <c t="s" s="2" r="A106">
+      <c t="s" s="3" r="A106">
         <v>1390</v>
       </c>
       <c t="s" s="6" r="B106">
@@ -21908,7 +21908,7 @@
       </c>
     </row>
     <row r="107">
-      <c t="s" s="2" r="A107">
+      <c t="s" s="3" r="A107">
         <v>1410</v>
       </c>
       <c t="s" s="6" r="B107">
@@ -21978,7 +21978,7 @@
       </c>
     </row>
     <row r="108">
-      <c t="s" s="2" r="A108">
+      <c t="s" s="3" r="A108">
         <v>1418</v>
       </c>
       <c t="s" s="6" r="B108">
@@ -22046,7 +22046,7 @@
       </c>
     </row>
     <row r="109">
-      <c t="s" s="2" r="A109">
+      <c t="s" s="3" r="A109">
         <v>1420</v>
       </c>
       <c t="s" s="6" r="B109">
@@ -22118,7 +22118,7 @@
       </c>
     </row>
     <row r="110">
-      <c t="s" s="2" r="A110">
+      <c t="s" s="3" r="A110">
         <v>1440</v>
       </c>
       <c t="s" s="6" r="B110">
@@ -22190,7 +22190,7 @@
       </c>
     </row>
     <row r="111">
-      <c t="s" s="2" r="A111">
+      <c t="s" s="3" r="A111">
         <v>1461</v>
       </c>
       <c t="s" s="6" r="B111">
@@ -22262,7 +22262,7 @@
       </c>
     </row>
     <row r="112">
-      <c t="s" s="2" r="A112">
+      <c t="s" s="3" r="A112">
         <v>1482</v>
       </c>
       <c t="s" s="6" r="B112">
@@ -22334,7 +22334,7 @@
       </c>
     </row>
     <row r="113">
-      <c t="s" s="2" r="A113">
+      <c t="s" s="3" r="A113">
         <v>1501</v>
       </c>
       <c t="s" s="6" r="B113">
@@ -22406,7 +22406,7 @@
       </c>
     </row>
     <row r="114">
-      <c t="s" s="2" r="A114">
+      <c t="s" s="3" r="A114">
         <v>1521</v>
       </c>
       <c t="s" s="6" r="B114">
@@ -22478,7 +22478,7 @@
       </c>
     </row>
     <row r="115">
-      <c t="s" s="2" r="A115">
+      <c t="s" s="3" r="A115">
         <v>1541</v>
       </c>
       <c t="s" s="6" r="B115">
@@ -22548,7 +22548,7 @@
       </c>
     </row>
     <row r="116">
-      <c t="s" s="2" r="A116">
+      <c t="s" s="3" r="A116">
         <v>1561</v>
       </c>
       <c t="s" s="6" r="B116">
@@ -22618,7 +22618,7 @@
       </c>
     </row>
     <row r="117">
-      <c t="s" s="2" r="A117">
+      <c t="s" s="3" r="A117">
         <v>1580</v>
       </c>
       <c t="s" s="6" r="B117">
@@ -22686,7 +22686,7 @@
       </c>
     </row>
     <row r="118">
-      <c t="s" s="2" r="A118">
+      <c t="s" s="3" r="A118">
         <v>1590</v>
       </c>
       <c t="s" s="6" r="B118">
@@ -22758,7 +22758,7 @@
       </c>
     </row>
     <row r="119">
-      <c t="s" s="2" r="A119">
+      <c t="s" s="3" r="A119">
         <v>1595</v>
       </c>
       <c t="s" s="6" r="B119">
@@ -22830,7 +22830,7 @@
       </c>
     </row>
     <row r="120">
-      <c t="s" s="2" r="A120">
+      <c t="s" s="3" r="A120">
         <v>1614</v>
       </c>
       <c t="s" s="6" r="B120">
@@ -22902,7 +22902,7 @@
       </c>
     </row>
     <row r="121">
-      <c t="s" s="2" r="A121">
+      <c t="s" s="3" r="A121">
         <v>1631</v>
       </c>
       <c t="s" s="6" r="B121">
@@ -22974,7 +22974,7 @@
       </c>
     </row>
     <row r="122">
-      <c t="s" s="2" r="A122">
+      <c t="s" s="3" r="A122">
         <v>1652</v>
       </c>
       <c t="s" s="6" r="B122">
@@ -23046,7 +23046,7 @@
       </c>
     </row>
     <row r="123">
-      <c t="s" s="2" r="A123">
+      <c t="s" s="3" r="A123">
         <v>1672</v>
       </c>
       <c t="s" s="6" r="B123">
@@ -23116,7 +23116,7 @@
       </c>
     </row>
     <row r="124">
-      <c t="s" s="2" r="A124">
+      <c t="s" s="3" r="A124">
         <v>1692</v>
       </c>
       <c t="s" s="6" r="B124">
@@ -23188,7 +23188,7 @@
       </c>
     </row>
     <row r="125">
-      <c t="s" s="2" r="A125">
+      <c t="s" s="3" r="A125">
         <v>1697</v>
       </c>
       <c t="s" s="6" r="B125">
@@ -23256,7 +23256,7 @@
       </c>
     </row>
     <row r="126">
-      <c t="s" s="2" r="A126">
+      <c t="s" s="3" r="A126">
         <v>1710</v>
       </c>
       <c t="s" s="6" r="B126">
@@ -23328,7 +23328,7 @@
       </c>
     </row>
     <row r="127">
-      <c t="s" s="2" r="A127">
+      <c t="s" s="3" r="A127">
         <v>1726</v>
       </c>
       <c t="s" s="6" r="B127">
@@ -23400,7 +23400,7 @@
       </c>
     </row>
     <row r="128">
-      <c t="s" s="2" r="A128">
+      <c t="s" s="3" r="A128">
         <v>1747</v>
       </c>
       <c t="s" s="6" r="B128">
@@ -23472,7 +23472,7 @@
       </c>
     </row>
     <row r="129">
-      <c t="s" s="2" r="A129">
+      <c t="s" s="3" r="A129">
         <v>1768</v>
       </c>
       <c t="s" s="6" r="B129">
@@ -23544,7 +23544,7 @@
       </c>
     </row>
     <row r="130">
-      <c t="s" s="2" r="A130">
+      <c t="s" s="3" r="A130">
         <v>1788</v>
       </c>
       <c t="s" s="6" r="B130">
@@ -23612,7 +23612,7 @@
       </c>
     </row>
     <row r="131">
-      <c t="s" s="2" r="A131">
+      <c t="s" s="3" r="A131">
         <v>1793</v>
       </c>
       <c t="s" s="6" r="B131">
@@ -23684,7 +23684,7 @@
       </c>
     </row>
     <row r="132">
-      <c t="s" s="2" r="A132">
+      <c t="s" s="3" r="A132">
         <v>1810</v>
       </c>
       <c t="s" s="6" r="B132">
@@ -23756,7 +23756,7 @@
       </c>
     </row>
     <row r="133">
-      <c t="s" s="2" r="A133">
+      <c t="s" s="3" r="A133">
         <v>1826</v>
       </c>
       <c t="s" s="6" r="B133">
@@ -23828,7 +23828,7 @@
       </c>
     </row>
     <row r="134">
-      <c t="s" s="2" r="A134">
+      <c t="s" s="3" r="A134">
         <v>1847</v>
       </c>
       <c t="s" s="6" r="B134">
@@ -23900,7 +23900,7 @@
       </c>
     </row>
     <row r="135">
-      <c t="s" s="2" r="A135">
+      <c t="s" s="3" r="A135">
         <v>1868</v>
       </c>
       <c t="s" s="6" r="B135">
@@ -23972,7 +23972,7 @@
       </c>
     </row>
     <row r="136">
-      <c t="s" s="2" r="A136">
+      <c t="s" s="3" r="A136">
         <v>1889</v>
       </c>
       <c t="s" s="6" r="B136">
@@ -24042,7 +24042,7 @@
       </c>
     </row>
     <row r="137">
-      <c t="s" s="2" r="A137">
+      <c t="s" s="3" r="A137">
         <v>1910</v>
       </c>
       <c t="s" s="6" r="B137">
@@ -24110,19 +24110,19 @@
       </c>
     </row>
     <row r="138">
-      <c t="s" s="2" r="A138">
+      <c t="s" s="3" r="A138">
         <v>1928</v>
       </c>
-      <c t="s" s="5" r="B138">
+      <c t="s" s="1" r="B138">
         <v>1929</v>
       </c>
-      <c t="s" s="5" r="C138">
+      <c t="s" s="1" r="C138">
         <v>1929</v>
       </c>
-      <c t="s" s="5" r="D138">
+      <c t="s" s="1" r="D138">
         <v>1929</v>
       </c>
-      <c t="s" s="5" r="E138">
+      <c t="s" s="1" r="E138">
         <v>1929</v>
       </c>
       <c t="s" s="6" r="F138">
@@ -24131,22 +24131,22 @@
       <c s="6" r="G138"/>
       <c s="6" r="H138"/>
       <c s="6" r="I138"/>
-      <c t="s" s="5" r="J138">
+      <c t="s" s="1" r="J138">
         <v>1929</v>
       </c>
       <c t="s" s="6" r="K138">
         <v>1930</v>
       </c>
       <c s="6" r="L138"/>
-      <c t="s" s="5" r="M138">
+      <c t="s" s="1" r="M138">
         <v>1929</v>
       </c>
-      <c t="s" s="5" r="N138">
+      <c t="s" s="1" r="N138">
         <v>1929</v>
       </c>
       <c s="6" r="O138"/>
       <c s="6" r="P138"/>
-      <c t="s" s="5" r="Q138">
+      <c t="s" s="1" r="Q138">
         <v>1929</v>
       </c>
       <c t="s" s="6" r="R138">
@@ -24158,7 +24158,7 @@
       <c t="s" s="6" r="T138">
         <v>1929</v>
       </c>
-      <c t="s" s="5" r="U138">
+      <c t="s" s="1" r="U138">
         <v>1929</v>
       </c>
       <c s="6" r="V138"/>
@@ -24171,12 +24171,12 @@
       <c t="s" s="6" r="Y138">
         <v>1929</v>
       </c>
-      <c t="s" s="5" r="Z138">
+      <c t="s" s="1" r="Z138">
         <v>1929</v>
       </c>
     </row>
     <row r="139">
-      <c t="s" s="2" r="A139">
+      <c t="s" s="3" r="A139">
         <v>1931</v>
       </c>
       <c t="s" s="6" r="B139">
@@ -24246,7 +24246,7 @@
       </c>
     </row>
     <row r="140">
-      <c t="s" s="2" r="A140">
+      <c t="s" s="3" r="A140">
         <v>1936</v>
       </c>
       <c t="s" s="6" r="B140">
@@ -24318,7 +24318,7 @@
       </c>
     </row>
     <row r="141">
-      <c t="s" s="2" r="A141">
+      <c t="s" s="3" r="A141">
         <v>1954</v>
       </c>
       <c t="s" s="6" r="B141">
@@ -24392,7 +24392,7 @@
       </c>
     </row>
     <row r="142">
-      <c t="s" s="2" r="A142">
+      <c t="s" s="3" r="A142">
         <v>1976</v>
       </c>
       <c t="s" s="6" r="B142">
@@ -24466,7 +24466,7 @@
       </c>
     </row>
     <row r="143">
-      <c t="s" s="2" r="A143">
+      <c t="s" s="3" r="A143">
         <v>1997</v>
       </c>
       <c t="s" s="6" r="B143">
@@ -24540,7 +24540,7 @@
       </c>
     </row>
     <row r="144">
-      <c t="s" s="2" r="A144">
+      <c t="s" s="3" r="A144">
         <v>2018</v>
       </c>
       <c t="s" s="6" r="B144">
@@ -24614,7 +24614,7 @@
       </c>
     </row>
     <row r="145">
-      <c t="s" s="2" r="A145">
+      <c t="s" s="3" r="A145">
         <v>2039</v>
       </c>
       <c t="s" s="6" r="B145">
@@ -24688,7 +24688,7 @@
       </c>
     </row>
     <row r="146">
-      <c t="s" s="2" r="A146">
+      <c t="s" s="3" r="A146">
         <v>2060</v>
       </c>
       <c t="s" s="6" r="B146">
@@ -24762,7 +24762,7 @@
       </c>
     </row>
     <row r="147">
-      <c t="s" s="2" r="A147">
+      <c t="s" s="3" r="A147">
         <v>2081</v>
       </c>
       <c t="s" s="6" r="B147">
@@ -24836,7 +24836,7 @@
       </c>
     </row>
     <row r="148">
-      <c t="s" s="2" r="A148">
+      <c t="s" s="3" r="A148">
         <v>2103</v>
       </c>
       <c t="s" s="6" r="B148">
@@ -24910,7 +24910,7 @@
       </c>
     </row>
     <row r="149">
-      <c t="s" s="2" r="A149">
+      <c t="s" s="3" r="A149">
         <v>2121</v>
       </c>
       <c t="s" s="6" r="B149">
@@ -24984,7 +24984,7 @@
       </c>
     </row>
     <row r="150">
-      <c t="s" s="2" r="A150">
+      <c t="s" s="3" r="A150">
         <v>2142</v>
       </c>
       <c t="s" s="6" r="B150">
@@ -25056,7 +25056,7 @@
       </c>
     </row>
     <row r="151">
-      <c t="s" s="2" r="A151">
+      <c t="s" s="3" r="A151">
         <v>2160</v>
       </c>
       <c t="s" s="6" r="B151">
@@ -25128,7 +25128,7 @@
       </c>
     </row>
     <row r="152">
-      <c t="s" s="2" r="A152">
+      <c t="s" s="3" r="A152">
         <v>2174</v>
       </c>
       <c t="s" s="6" r="B152">
@@ -25200,7 +25200,7 @@
       </c>
     </row>
     <row r="153">
-      <c t="s" s="2" r="A153">
+      <c t="s" s="3" r="A153">
         <v>2189</v>
       </c>
       <c t="s" s="6" r="B153">
@@ -25272,7 +25272,7 @@
       </c>
     </row>
     <row r="154">
-      <c t="s" s="2" r="A154">
+      <c t="s" s="3" r="A154">
         <v>2205</v>
       </c>
       <c t="s" s="6" r="B154">
@@ -25346,7 +25346,7 @@
       </c>
     </row>
     <row r="155">
-      <c t="s" s="2" r="A155">
+      <c t="s" s="3" r="A155">
         <v>2227</v>
       </c>
       <c t="s" s="6" r="B155">
@@ -25420,7 +25420,7 @@
       </c>
     </row>
     <row r="156">
-      <c t="s" s="2" r="A156">
+      <c t="s" s="3" r="A156">
         <v>2244</v>
       </c>
       <c t="s" s="6" r="B156">
@@ -25490,7 +25490,7 @@
       </c>
     </row>
     <row r="157">
-      <c t="s" s="2" r="A157">
+      <c t="s" s="3" r="A157">
         <v>2248</v>
       </c>
       <c t="s" s="6" r="B157">
@@ -25564,7 +25564,7 @@
       </c>
     </row>
     <row r="158">
-      <c t="s" s="2" r="A158">
+      <c t="s" s="3" r="A158">
         <v>2255</v>
       </c>
       <c t="s" s="6" r="B158">
@@ -25638,7 +25638,7 @@
       </c>
     </row>
     <row r="159">
-      <c t="s" s="2" r="A159">
+      <c t="s" s="3" r="A159">
         <v>2274</v>
       </c>
       <c t="s" s="6" r="B159">
@@ -25708,7 +25708,7 @@
       </c>
     </row>
     <row r="160">
-      <c t="s" s="2" r="A160">
+      <c t="s" s="3" r="A160">
         <v>2290</v>
       </c>
       <c t="s" s="6" r="B160">
@@ -25778,7 +25778,7 @@
       </c>
     </row>
     <row r="161">
-      <c t="s" s="2" r="A161">
+      <c t="s" s="3" r="A161">
         <v>2309</v>
       </c>
       <c t="s" s="6" r="B161">
@@ -25852,7 +25852,7 @@
       </c>
     </row>
     <row r="162">
-      <c t="s" s="2" r="A162">
+      <c t="s" s="3" r="A162">
         <v>2331</v>
       </c>
       <c t="s" s="6" r="B162">
@@ -25926,7 +25926,7 @@
       </c>
     </row>
     <row r="163">
-      <c t="s" s="2" r="A163">
+      <c t="s" s="3" r="A163">
         <v>2353</v>
       </c>
       <c t="s" s="6" r="B163">
@@ -26000,7 +26000,7 @@
       </c>
     </row>
     <row r="164">
-      <c t="s" s="2" r="A164">
+      <c t="s" s="3" r="A164">
         <v>2373</v>
       </c>
       <c t="s" s="6" r="B164">
@@ -26074,7 +26074,7 @@
       </c>
     </row>
     <row r="165">
-      <c t="s" s="2" r="A165">
+      <c t="s" s="3" r="A165">
         <v>2396</v>
       </c>
       <c t="s" s="6" r="B165">
@@ -26148,7 +26148,7 @@
       </c>
     </row>
     <row r="166">
-      <c t="s" s="2" r="A166">
+      <c t="s" s="3" r="A166">
         <v>2418</v>
       </c>
       <c t="s" s="6" r="B166">
@@ -26222,7 +26222,7 @@
       </c>
     </row>
     <row r="167">
-      <c t="s" s="2" r="A167">
+      <c t="s" s="3" r="A167">
         <v>2440</v>
       </c>
       <c t="s" s="6" r="B167">
@@ -26296,7 +26296,7 @@
       </c>
     </row>
     <row r="168">
-      <c t="s" s="2" r="A168">
+      <c t="s" s="3" r="A168">
         <v>2462</v>
       </c>
       <c t="s" s="6" r="B168">
@@ -26368,7 +26368,7 @@
       </c>
     </row>
     <row r="169">
-      <c t="s" s="2" r="A169">
+      <c t="s" s="3" r="A169">
         <v>2464</v>
       </c>
       <c t="s" s="6" r="B169">
@@ -26440,7 +26440,7 @@
       </c>
     </row>
     <row r="170">
-      <c t="s" s="2" r="A170">
+      <c t="s" s="3" r="A170">
         <v>2466</v>
       </c>
       <c t="s" s="6" r="B170">
@@ -26512,7 +26512,7 @@
       </c>
     </row>
     <row r="171">
-      <c t="s" s="2" r="A171">
+      <c t="s" s="3" r="A171">
         <v>2468</v>
       </c>
       <c t="s" s="6" r="B171">
@@ -26584,7 +26584,7 @@
       </c>
     </row>
     <row r="172">
-      <c t="s" s="2" r="A172">
+      <c t="s" s="3" r="A172">
         <v>2489</v>
       </c>
       <c t="s" s="6" r="B172">
@@ -26656,7 +26656,7 @@
       </c>
     </row>
     <row r="173">
-      <c t="s" s="2" r="A173">
+      <c t="s" s="3" r="A173">
         <v>2510</v>
       </c>
       <c t="s" s="6" r="B173">
@@ -26730,7 +26730,7 @@
       </c>
     </row>
     <row r="174">
-      <c t="s" s="2" r="A174">
+      <c t="s" s="3" r="A174">
         <v>2532</v>
       </c>
       <c t="s" s="6" r="B174">
@@ -26806,7 +26806,7 @@
       </c>
     </row>
     <row r="175">
-      <c t="s" s="2" r="A175">
+      <c t="s" s="3" r="A175">
         <v>2555</v>
       </c>
       <c t="s" s="6" r="B175">
@@ -26882,7 +26882,7 @@
       </c>
     </row>
     <row r="176">
-      <c t="s" s="2" r="A176">
+      <c t="s" s="3" r="A176">
         <v>2578</v>
       </c>
       <c t="s" s="6" r="B176">
@@ -26958,7 +26958,7 @@
       </c>
     </row>
     <row r="177">
-      <c t="s" s="2" r="A177">
+      <c t="s" s="3" r="A177">
         <v>2602</v>
       </c>
       <c t="s" s="6" r="B177">
@@ -27034,7 +27034,7 @@
       </c>
     </row>
     <row r="178">
-      <c t="s" s="2" r="A178">
+      <c t="s" s="3" r="A178">
         <v>2625</v>
       </c>
       <c t="s" s="6" r="B178">
@@ -27110,7 +27110,7 @@
       </c>
     </row>
     <row r="179">
-      <c t="s" s="2" r="A179">
+      <c t="s" s="3" r="A179">
         <v>2648</v>
       </c>
       <c t="s" s="6" r="B179">
@@ -27186,7 +27186,7 @@
       </c>
     </row>
     <row r="180">
-      <c t="s" s="2" r="A180">
+      <c t="s" s="3" r="A180">
         <v>2670</v>
       </c>
       <c t="s" s="6" r="B180">
@@ -27262,7 +27262,7 @@
       </c>
     </row>
     <row r="181">
-      <c t="s" s="2" r="A181">
+      <c t="s" s="3" r="A181">
         <v>2677</v>
       </c>
       <c t="s" s="6" r="B181">
@@ -27338,7 +27338,7 @@
       </c>
     </row>
     <row r="182">
-      <c t="s" s="2" r="A182">
+      <c t="s" s="3" r="A182">
         <v>2699</v>
       </c>
       <c t="s" s="6" r="B182">
@@ -27414,7 +27414,7 @@
       </c>
     </row>
     <row r="183">
-      <c t="s" s="2" r="A183">
+      <c t="s" s="3" r="A183">
         <v>2721</v>
       </c>
       <c t="s" s="6" r="B183">
@@ -27490,7 +27490,7 @@
       </c>
     </row>
     <row r="184">
-      <c t="s" s="2" r="A184">
+      <c t="s" s="3" r="A184">
         <v>2743</v>
       </c>
       <c t="s" s="6" r="B184">
@@ -27566,7 +27566,7 @@
       </c>
     </row>
     <row r="185">
-      <c t="s" s="2" r="A185">
+      <c t="s" s="3" r="A185">
         <v>2766</v>
       </c>
       <c t="s" s="6" r="B185">
@@ -27642,7 +27642,7 @@
       </c>
     </row>
     <row r="186">
-      <c t="s" s="2" r="A186">
+      <c t="s" s="3" r="A186">
         <v>2790</v>
       </c>
       <c t="s" s="6" r="B186">
@@ -27718,7 +27718,7 @@
       </c>
     </row>
     <row r="187">
-      <c t="s" s="2" r="A187">
+      <c t="s" s="3" r="A187">
         <v>2814</v>
       </c>
       <c t="s" s="6" r="B187">
@@ -27792,7 +27792,7 @@
       </c>
     </row>
     <row r="188">
-      <c t="s" s="2" r="A188">
+      <c t="s" s="3" r="A188">
         <v>2836</v>
       </c>
       <c t="s" s="6" r="B188">
@@ -27868,7 +27868,7 @@
       </c>
     </row>
     <row r="189">
-      <c t="s" s="2" r="A189">
+      <c t="s" s="3" r="A189">
         <v>2860</v>
       </c>
       <c t="s" s="6" r="B189">
@@ -27944,7 +27944,7 @@
       </c>
     </row>
     <row r="190">
-      <c t="s" s="2" r="A190">
+      <c t="s" s="3" r="A190">
         <v>2884</v>
       </c>
       <c t="s" s="6" r="B190">
@@ -28020,7 +28020,7 @@
       </c>
     </row>
     <row r="191">
-      <c t="s" s="2" r="A191">
+      <c t="s" s="3" r="A191">
         <v>2893</v>
       </c>
       <c t="s" s="6" r="B191">
@@ -28096,7 +28096,7 @@
       </c>
     </row>
     <row r="192">
-      <c t="s" s="2" r="A192">
+      <c t="s" s="3" r="A192">
         <v>2913</v>
       </c>
       <c t="s" s="6" r="B192">
@@ -28170,7 +28170,7 @@
       </c>
     </row>
     <row r="193">
-      <c t="s" s="2" r="A193">
+      <c t="s" s="3" r="A193">
         <v>2917</v>
       </c>
       <c t="s" s="6" r="B193">
@@ -28244,7 +28244,7 @@
       </c>
     </row>
     <row r="194">
-      <c t="s" s="2" r="A194">
+      <c t="s" s="3" r="A194">
         <v>2920</v>
       </c>
       <c t="s" s="6" r="B194">
@@ -28320,7 +28320,7 @@
       </c>
     </row>
     <row r="195">
-      <c t="s" s="2" r="A195">
+      <c t="s" s="3" r="A195">
         <v>2942</v>
       </c>
       <c t="s" s="6" r="B195">
@@ -28396,7 +28396,7 @@
       </c>
     </row>
     <row r="196">
-      <c t="s" s="2" r="A196">
+      <c t="s" s="3" r="A196">
         <v>2949</v>
       </c>
       <c t="s" s="6" r="B196">
@@ -28472,7 +28472,7 @@
       </c>
     </row>
     <row r="197">
-      <c t="s" s="2" r="A197">
+      <c t="s" s="3" r="A197">
         <v>2972</v>
       </c>
       <c t="s" s="6" r="B197">
@@ -28548,7 +28548,7 @@
       </c>
     </row>
     <row r="198">
-      <c t="s" s="2" r="A198">
+      <c t="s" s="3" r="A198">
         <v>2993</v>
       </c>
       <c t="s" s="6" r="B198">
@@ -28624,7 +28624,7 @@
       </c>
     </row>
     <row r="199">
-      <c t="s" s="2" r="A199">
+      <c t="s" s="3" r="A199">
         <v>3015</v>
       </c>
       <c t="s" s="6" r="B199">
@@ -28704,7 +28704,7 @@
       </c>
     </row>
     <row r="200">
-      <c t="s" s="2" r="A200">
+      <c t="s" s="3" r="A200">
         <v>3039</v>
       </c>
       <c t="s" s="6" r="B200">
@@ -28784,7 +28784,7 @@
       </c>
     </row>
     <row r="201">
-      <c t="s" s="2" r="A201">
+      <c t="s" s="3" r="A201">
         <v>3059</v>
       </c>
       <c t="s" s="6" r="B201">
@@ -28862,7 +28862,7 @@
       </c>
     </row>
     <row r="202">
-      <c t="s" s="2" r="A202">
+      <c t="s" s="3" r="A202">
         <v>3078</v>
       </c>
       <c t="s" s="6" r="B202">
@@ -28942,7 +28942,7 @@
       </c>
     </row>
     <row r="203">
-      <c t="s" s="2" r="A203">
+      <c t="s" s="3" r="A203">
         <v>3104</v>
       </c>
       <c t="s" s="6" r="B203">
@@ -29022,7 +29022,7 @@
       </c>
     </row>
     <row r="204">
-      <c t="s" s="2" r="A204">
+      <c t="s" s="3" r="A204">
         <v>3129</v>
       </c>
       <c t="s" s="6" r="B204">
@@ -29102,7 +29102,7 @@
       </c>
     </row>
     <row r="205">
-      <c t="s" s="2" r="A205">
+      <c t="s" s="3" r="A205">
         <v>3152</v>
       </c>
       <c t="s" s="6" r="B205">
@@ -29178,7 +29178,7 @@
       </c>
     </row>
     <row r="206">
-      <c t="s" s="2" r="A206">
+      <c t="s" s="3" r="A206">
         <v>3173</v>
       </c>
       <c t="s" s="6" r="B206">
@@ -29258,7 +29258,7 @@
       </c>
     </row>
     <row r="207">
-      <c t="s" s="2" r="A207">
+      <c t="s" s="3" r="A207">
         <v>3198</v>
       </c>
       <c t="s" s="6" r="B207">
@@ -29334,7 +29334,7 @@
       </c>
     </row>
     <row r="208">
-      <c t="s" s="2" r="A208">
+      <c t="s" s="3" r="A208">
         <v>3222</v>
       </c>
       <c t="s" s="6" r="B208">
@@ -29412,7 +29412,7 @@
       </c>
     </row>
     <row r="209">
-      <c t="s" s="2" r="A209">
+      <c t="s" s="3" r="A209">
         <v>3238</v>
       </c>
       <c t="s" s="6" r="B209">
@@ -29490,7 +29490,7 @@
       </c>
     </row>
     <row r="210">
-      <c t="s" s="2" r="A210">
+      <c t="s" s="3" r="A210">
         <v>3255</v>
       </c>
       <c t="s" s="6" r="B210">
@@ -29570,7 +29570,7 @@
       </c>
     </row>
     <row r="211">
-      <c t="s" s="2" r="A211">
+      <c t="s" s="3" r="A211">
         <v>3279</v>
       </c>
       <c t="s" s="6" r="B211">
@@ -29648,7 +29648,7 @@
       </c>
     </row>
     <row r="212">
-      <c t="s" s="2" r="A212">
+      <c t="s" s="3" r="A212">
         <v>3298</v>
       </c>
       <c t="s" s="6" r="B212">
@@ -29728,7 +29728,7 @@
       </c>
     </row>
     <row r="213">
-      <c t="s" s="2" r="A213">
+      <c t="s" s="3" r="A213">
         <v>3324</v>
       </c>
       <c t="s" s="6" r="B213">
@@ -29806,7 +29806,7 @@
       </c>
     </row>
     <row r="214">
-      <c t="s" s="2" r="A214">
+      <c t="s" s="3" r="A214">
         <v>3342</v>
       </c>
       <c t="s" s="6" r="B214">
@@ -29884,7 +29884,7 @@
       </c>
     </row>
     <row r="215">
-      <c t="s" s="2" r="A215">
+      <c t="s" s="3" r="A215">
         <v>3357</v>
       </c>
       <c t="s" s="6" r="B215">
@@ -29958,7 +29958,7 @@
       </c>
     </row>
     <row r="216">
-      <c t="s" s="2" r="A216">
+      <c t="s" s="3" r="A216">
         <v>3376</v>
       </c>
       <c t="s" s="6" r="B216">
@@ -30034,7 +30034,7 @@
       </c>
     </row>
     <row r="217">
-      <c t="s" s="2" r="A217">
+      <c t="s" s="3" r="A217">
         <v>3400</v>
       </c>
       <c t="s" s="6" r="B217">
@@ -30080,7 +30080,7 @@
       </c>
     </row>
     <row r="218">
-      <c t="s" s="2" r="A218">
+      <c t="s" s="3" r="A218">
         <v>3405</v>
       </c>
       <c t="s" s="6" r="B218">
@@ -30158,7 +30158,7 @@
       </c>
     </row>
     <row r="219">
-      <c t="s" s="2" r="A219">
+      <c t="s" s="3" r="A219">
         <v>3430</v>
       </c>
       <c t="s" s="6" r="B219">
@@ -30238,7 +30238,7 @@
       </c>
     </row>
     <row r="220">
-      <c t="s" s="2" r="A220">
+      <c t="s" s="3" r="A220">
         <v>3456</v>
       </c>
       <c t="s" s="6" r="B220">
@@ -30318,7 +30318,7 @@
       </c>
     </row>
     <row r="221">
-      <c t="s" s="2" r="A221">
+      <c t="s" s="3" r="A221">
         <v>3482</v>
       </c>
       <c t="s" s="6" r="B221">
@@ -30396,7 +30396,7 @@
       </c>
     </row>
     <row r="222">
-      <c t="s" s="2" r="A222">
+      <c t="s" s="3" r="A222">
         <v>3507</v>
       </c>
       <c t="s" s="6" r="B222">
@@ -30474,7 +30474,7 @@
       </c>
     </row>
     <row r="223">
-      <c t="s" s="2" r="A223">
+      <c t="s" s="3" r="A223">
         <v>3532</v>
       </c>
       <c t="s" s="6" r="B223">
@@ -30552,7 +30552,7 @@
       </c>
     </row>
     <row r="224">
-      <c t="s" s="2" r="A224">
+      <c t="s" s="3" r="A224">
         <v>3557</v>
       </c>
       <c t="s" s="6" r="B224">
@@ -30632,7 +30632,7 @@
       </c>
     </row>
     <row r="225">
-      <c t="s" s="2" r="A225">
+      <c t="s" s="3" r="A225">
         <v>3567</v>
       </c>
       <c t="s" s="6" r="B225">
@@ -30710,7 +30710,7 @@
       </c>
     </row>
     <row r="226">
-      <c t="s" s="2" r="A226">
+      <c t="s" s="3" r="A226">
         <v>3592</v>
       </c>
       <c t="s" s="6" r="B226">
@@ -30790,7 +30790,7 @@
       </c>
     </row>
     <row r="227">
-      <c t="s" s="2" r="A227">
+      <c t="s" s="3" r="A227">
         <v>3618</v>
       </c>
       <c t="s" s="6" r="B227">
@@ -30868,7 +30868,7 @@
       </c>
     </row>
     <row r="228">
-      <c t="s" s="2" r="A228">
+      <c t="s" s="3" r="A228">
         <v>3643</v>
       </c>
       <c t="s" s="6" r="B228">
@@ -30948,7 +30948,7 @@
       </c>
     </row>
     <row r="229">
-      <c t="s" s="2" r="A229">
+      <c t="s" s="3" r="A229">
         <v>3657</v>
       </c>
       <c t="s" s="6" r="B229">
@@ -31026,7 +31026,7 @@
       </c>
     </row>
     <row r="230">
-      <c t="s" s="2" r="A230">
+      <c t="s" s="3" r="A230">
         <v>3660</v>
       </c>
       <c t="s" s="6" r="B230">
@@ -31106,7 +31106,7 @@
       </c>
     </row>
     <row r="231">
-      <c t="s" s="2" r="A231">
+      <c t="s" s="3" r="A231">
         <v>3663</v>
       </c>
       <c t="s" s="6" r="B231">
@@ -31186,7 +31186,7 @@
       </c>
     </row>
     <row r="232">
-      <c t="s" s="2" r="A232">
+      <c t="s" s="3" r="A232">
         <v>3666</v>
       </c>
       <c t="s" s="6" r="B232">
@@ -31266,7 +31266,7 @@
       </c>
     </row>
     <row r="233">
-      <c t="s" s="2" r="A233">
+      <c t="s" s="3" r="A233">
         <v>3669</v>
       </c>
       <c t="s" s="6" r="B233">
@@ -31346,7 +31346,7 @@
       </c>
     </row>
     <row r="234">
-      <c t="s" s="2" r="A234">
+      <c t="s" s="3" r="A234">
         <v>3681</v>
       </c>
       <c t="s" s="6" r="B234">
@@ -31424,7 +31424,7 @@
       </c>
     </row>
     <row r="235">
-      <c t="s" s="2" r="A235">
+      <c t="s" s="3" r="A235">
         <v>3706</v>
       </c>
       <c t="s" s="6" r="B235">
@@ -31504,7 +31504,7 @@
       </c>
     </row>
     <row r="236">
-      <c t="s" s="2" r="A236">
+      <c t="s" s="3" r="A236">
         <v>3732</v>
       </c>
       <c t="s" s="6" r="B236">
@@ -31584,7 +31584,7 @@
       </c>
     </row>
     <row r="237">
-      <c t="s" s="2" r="A237">
+      <c t="s" s="3" r="A237">
         <v>3758</v>
       </c>
       <c t="s" s="6" r="B237">
@@ -31664,7 +31664,7 @@
       </c>
     </row>
     <row r="238">
-      <c t="s" s="2" r="A238">
+      <c t="s" s="3" r="A238">
         <v>3784</v>
       </c>
       <c t="s" s="6" r="B238">
@@ -31742,7 +31742,7 @@
       </c>
     </row>
     <row r="239">
-      <c t="s" s="2" r="A239">
+      <c t="s" s="3" r="A239">
         <v>3809</v>
       </c>
       <c t="s" s="6" r="B239">
@@ -31822,7 +31822,7 @@
       </c>
     </row>
     <row r="240">
-      <c t="s" s="2" r="A240">
+      <c t="s" s="3" r="A240">
         <v>3835</v>
       </c>
       <c t="s" s="6" r="B240">
@@ -31902,7 +31902,7 @@
       </c>
     </row>
     <row r="241">
-      <c t="s" s="2" r="A241">
+      <c t="s" s="3" r="A241">
         <v>3860</v>
       </c>
       <c t="s" s="6" r="B241">
@@ -31982,7 +31982,7 @@
       </c>
     </row>
     <row r="242">
-      <c t="s" s="2" r="A242">
+      <c t="s" s="3" r="A242">
         <v>3872</v>
       </c>
       <c t="s" s="6" r="B242">
@@ -32060,7 +32060,7 @@
       </c>
     </row>
     <row r="243">
-      <c t="s" s="2" r="A243">
+      <c t="s" s="3" r="A243">
         <v>3884</v>
       </c>
       <c t="s" s="6" r="B243">
@@ -32138,7 +32138,7 @@
       </c>
     </row>
     <row r="244">
-      <c t="s" s="2" r="A244">
+      <c t="s" s="3" r="A244">
         <v>3888</v>
       </c>
       <c t="s" s="6" r="B244">
@@ -32218,7 +32218,7 @@
       </c>
     </row>
     <row r="245">
-      <c t="s" s="2" r="A245">
+      <c t="s" s="3" r="A245">
         <v>3912</v>
       </c>
       <c t="s" s="6" r="B245">
@@ -32296,7 +32296,7 @@
       </c>
     </row>
     <row r="246">
-      <c t="s" s="2" r="A246">
+      <c t="s" s="3" r="A246">
         <v>3928</v>
       </c>
       <c t="s" s="6" r="B246">
@@ -32374,7 +32374,7 @@
       </c>
     </row>
     <row r="247">
-      <c t="s" s="2" r="A247">
+      <c t="s" s="3" r="A247">
         <v>3953</v>
       </c>
       <c t="s" s="6" r="B247">
@@ -32452,7 +32452,7 @@
       </c>
     </row>
     <row r="248">
-      <c t="s" s="2" r="A248">
+      <c t="s" s="3" r="A248">
         <v>3975</v>
       </c>
       <c t="s" s="6" r="B248">
@@ -32530,7 +32530,7 @@
       </c>
     </row>
     <row r="249">
-      <c t="s" s="2" r="A249">
+      <c t="s" s="3" r="A249">
         <v>4000</v>
       </c>
       <c t="s" s="6" r="B249">
@@ -32608,7 +32608,7 @@
       </c>
     </row>
     <row r="250">
-      <c t="s" s="2" r="A250">
+      <c t="s" s="3" r="A250">
         <v>4016</v>
       </c>
       <c t="s" s="6" r="B250">
@@ -32682,7 +32682,7 @@
       </c>
     </row>
     <row r="251">
-      <c t="s" s="2" r="A251">
+      <c t="s" s="3" r="A251">
         <v>4019</v>
       </c>
       <c t="s" s="6" r="B251">
@@ -32756,7 +32756,7 @@
       </c>
     </row>
     <row r="252">
-      <c t="s" s="2" r="A252">
+      <c t="s" s="3" r="A252">
         <v>4022</v>
       </c>
       <c t="s" s="6" r="B252">
@@ -32830,7 +32830,7 @@
       </c>
     </row>
     <row r="253">
-      <c t="s" s="2" r="A253">
+      <c t="s" s="3" r="A253">
         <v>4025</v>
       </c>
       <c t="s" s="6" r="B253">
@@ -32908,159 +32908,159 @@
       </c>
     </row>
     <row r="254">
-      <c t="s" s="2" r="A254">
+      <c t="s" s="3" r="A254">
         <v>4031</v>
       </c>
-      <c t="s" s="5" r="B254">
+      <c t="s" s="1" r="B254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="C254">
+      <c t="s" s="1" r="C254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="D254">
+      <c t="s" s="1" r="D254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="E254">
+      <c t="s" s="1" r="E254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="F254">
+      <c t="s" s="1" r="F254">
         <v>4032</v>
       </c>
       <c t="s" s="6" r="G254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="H254">
+      <c t="s" s="1" r="H254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="I254">
+      <c t="s" s="1" r="I254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="J254">
+      <c t="s" s="1" r="J254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="K254">
+      <c t="s" s="1" r="K254">
         <v>4033</v>
       </c>
-      <c t="s" s="5" r="L254">
+      <c t="s" s="1" r="L254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="M254">
+      <c t="s" s="1" r="M254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="N254">
+      <c t="s" s="1" r="N254">
         <v>4032</v>
       </c>
       <c t="s" s="6" r="O254">
         <v>4032</v>
       </c>
       <c s="6" r="P254"/>
-      <c t="s" s="5" r="Q254">
+      <c t="s" s="1" r="Q254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="R254">
+      <c t="s" s="1" r="R254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="S254">
+      <c t="s" s="1" r="S254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="T254">
+      <c t="s" s="1" r="T254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="U254">
+      <c t="s" s="1" r="U254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="V254">
+      <c t="s" s="1" r="V254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="W254">
+      <c t="s" s="1" r="W254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="X254">
+      <c t="s" s="1" r="X254">
         <v>4032</v>
       </c>
       <c t="s" s="6" r="Y254">
         <v>4032</v>
       </c>
-      <c t="s" s="5" r="Z254">
+      <c t="s" s="1" r="Z254">
         <v>4032</v>
       </c>
     </row>
     <row r="255">
-      <c t="s" s="2" r="A255">
+      <c t="s" s="3" r="A255">
         <v>4034</v>
       </c>
-      <c t="s" s="5" r="B255">
+      <c t="s" s="1" r="B255">
         <v>4035</v>
       </c>
-      <c t="s" s="5" r="C255">
+      <c t="s" s="1" r="C255">
         <v>4035</v>
       </c>
-      <c t="s" s="5" r="D255">
+      <c t="s" s="1" r="D255">
         <v>4035</v>
       </c>
-      <c t="s" s="5" r="E255">
+      <c t="s" s="1" r="E255">
         <v>4035</v>
       </c>
-      <c t="s" s="5" r="F255">
+      <c t="s" s="1" r="F255">
         <v>4035</v>
       </c>
       <c t="s" s="6" r="G255">
         <v>4035</v>
       </c>
-      <c t="s" s="5" r="H255">
+      <c t="s" s="1" r="H255">
         <v>4035</v>
       </c>
       <c s="6" r="I255"/>
-      <c t="s" s="5" r="J255">
+      <c t="s" s="1" r="J255">
         <v>4035</v>
       </c>
       <c t="s" s="6" r="K255">
         <v>4036</v>
       </c>
-      <c t="s" s="5" r="L255">
+      <c t="s" s="1" r="L255">
         <v>4035</v>
       </c>
-      <c t="s" s="5" r="M255">
+      <c t="s" s="1" r="M255">
         <v>4035</v>
       </c>
-      <c t="s" s="5" r="N255">
+      <c t="s" s="1" r="N255">
         <v>4035</v>
       </c>
       <c s="6" r="O255"/>
       <c s="6" r="P255"/>
-      <c t="s" s="5" r="Q255">
+      <c t="s" s="1" r="Q255">
         <v>4035</v>
       </c>
-      <c t="s" s="5" r="R255">
+      <c t="s" s="1" r="R255">
         <v>4035</v>
       </c>
-      <c t="s" s="5" r="S255">
+      <c t="s" s="1" r="S255">
         <v>4037</v>
       </c>
-      <c t="s" s="5" r="T255">
+      <c t="s" s="1" r="T255">
         <v>4035</v>
       </c>
-      <c t="s" s="5" r="U255">
+      <c t="s" s="1" r="U255">
         <v>4038</v>
       </c>
-      <c t="s" s="5" r="V255">
+      <c t="s" s="1" r="V255">
         <v>4035</v>
       </c>
-      <c t="s" s="5" r="W255">
+      <c t="s" s="1" r="W255">
         <v>4035</v>
       </c>
-      <c t="s" s="5" r="X255">
+      <c t="s" s="1" r="X255">
         <v>4035</v>
       </c>
       <c t="s" s="6" r="Y255">
         <v>4035</v>
       </c>
-      <c t="s" s="5" r="Z255">
+      <c t="s" s="1" r="Z255">
         <v>4035</v>
       </c>
     </row>
     <row r="256">
-      <c t="s" s="2" r="A256">
+      <c t="s" s="3" r="A256">
         <v>4039</v>
       </c>
       <c t="s" s="6" r="B256">
@@ -33134,7 +33134,7 @@
       </c>
     </row>
     <row r="257">
-      <c t="s" s="2" r="A257">
+      <c t="s" s="3" r="A257">
         <v>4042</v>
       </c>
       <c t="s" s="6" r="B257">
@@ -33208,7 +33208,7 @@
       </c>
     </row>
     <row r="258">
-      <c t="s" s="2" r="A258">
+      <c t="s" s="3" r="A258">
         <v>4045</v>
       </c>
       <c t="s" s="6" r="B258">
@@ -33282,106 +33282,106 @@
       </c>
     </row>
     <row r="259">
-      <c t="s" s="2" r="A259">
+      <c t="s" s="3" r="A259">
         <v>4048</v>
       </c>
-      <c t="s" s="5" r="B259">
+      <c t="s" s="1" r="B259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="C259">
+      <c t="s" s="1" r="C259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="D259">
+      <c t="s" s="1" r="D259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="E259">
+      <c t="s" s="1" r="E259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="F259">
+      <c t="s" s="1" r="F259">
         <v>4049</v>
       </c>
       <c t="s" s="6" r="G259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="H259">
+      <c t="s" s="1" r="H259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="I259">
+      <c t="s" s="1" r="I259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="J259">
+      <c t="s" s="1" r="J259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="K259">
+      <c t="s" s="1" r="K259">
         <v>4050</v>
       </c>
-      <c t="s" s="5" r="L259">
+      <c t="s" s="1" r="L259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="M259">
+      <c t="s" s="1" r="M259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="N259">
+      <c t="s" s="1" r="N259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="O259">
+      <c t="s" s="1" r="O259">
         <v>4051</v>
       </c>
       <c s="6" r="P259"/>
-      <c t="s" s="5" r="Q259">
+      <c t="s" s="1" r="Q259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="R259">
+      <c t="s" s="1" r="R259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="S259">
+      <c t="s" s="1" r="S259">
         <v>4052</v>
       </c>
-      <c t="s" s="5" r="T259">
+      <c t="s" s="1" r="T259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="U259">
+      <c t="s" s="1" r="U259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="V259">
+      <c t="s" s="1" r="V259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="W259">
+      <c t="s" s="1" r="W259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="X259">
+      <c t="s" s="1" r="X259">
         <v>4049</v>
       </c>
       <c t="s" s="6" r="Y259">
         <v>4049</v>
       </c>
-      <c t="s" s="5" r="Z259">
+      <c t="s" s="1" r="Z259">
         <v>4049</v>
       </c>
     </row>
     <row r="260">
-      <c t="s" s="2" r="A260">
+      <c t="s" s="3" r="A260">
         <v>4053</v>
       </c>
-      <c t="s" s="5" r="B260">
+      <c t="s" s="1" r="B260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="C260">
+      <c t="s" s="1" r="C260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="D260">
+      <c t="s" s="1" r="D260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="E260">
+      <c t="s" s="1" r="E260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="F260">
+      <c t="s" s="1" r="F260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="G260">
+      <c t="s" s="1" r="G260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="H260">
+      <c t="s" s="1" r="H260">
         <v>4054</v>
       </c>
       <c s="6" r="I260"/>
@@ -33389,50 +33389,50 @@
       <c t="s" s="6" r="K260">
         <v>4055</v>
       </c>
-      <c t="s" s="5" r="L260">
+      <c t="s" s="1" r="L260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="M260">
+      <c t="s" s="1" r="M260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="N260">
+      <c t="s" s="1" r="N260">
         <v>4054</v>
       </c>
       <c s="6" r="O260"/>
       <c s="6" r="P260"/>
-      <c t="s" s="5" r="Q260">
+      <c t="s" s="1" r="Q260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="R260">
+      <c t="s" s="1" r="R260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="S260">
+      <c t="s" s="1" r="S260">
         <v>4052</v>
       </c>
-      <c t="s" s="5" r="T260">
+      <c t="s" s="1" r="T260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="U260">
+      <c t="s" s="1" r="U260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="V260">
+      <c t="s" s="1" r="V260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="W260">
+      <c t="s" s="1" r="W260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="X260">
+      <c t="s" s="1" r="X260">
         <v>4054</v>
       </c>
       <c t="s" s="6" r="Y260">
         <v>4054</v>
       </c>
-      <c t="s" s="5" r="Z260">
+      <c t="s" s="1" r="Z260">
         <v>4054</v>
       </c>
     </row>
     <row r="261">
-      <c t="s" s="2" r="A261">
+      <c t="s" s="3" r="A261">
         <v>4056</v>
       </c>
       <c t="s" s="6" r="B261">
@@ -33512,7 +33512,7 @@
       </c>
     </row>
     <row r="262">
-      <c t="s" s="2" r="A262">
+      <c t="s" s="3" r="A262">
         <v>4081</v>
       </c>
       <c t="s" s="6" r="B262">
@@ -33590,7 +33590,7 @@
       </c>
     </row>
     <row r="263">
-      <c t="s" s="2" r="A263">
+      <c t="s" s="3" r="A263">
         <v>4101</v>
       </c>
       <c t="s" s="6" r="B263">
@@ -33668,7 +33668,7 @@
       </c>
     </row>
     <row r="264">
-      <c t="s" s="2" r="A264">
+      <c t="s" s="3" r="A264">
         <v>4104</v>
       </c>
       <c t="s" s="6" r="B264">
@@ -33746,7 +33746,7 @@
       </c>
     </row>
     <row r="265">
-      <c t="s" s="2" r="A265">
+      <c t="s" s="3" r="A265">
         <v>4109</v>
       </c>
       <c t="s" s="6" r="B265">
@@ -33824,7 +33824,7 @@
       </c>
     </row>
     <row r="266">
-      <c t="s" s="2" r="A266">
+      <c t="s" s="3" r="A266">
         <v>4114</v>
       </c>
       <c t="s" s="6" r="B266">
@@ -33902,7 +33902,7 @@
       </c>
     </row>
     <row r="267">
-      <c t="s" s="2" r="A267">
+      <c t="s" s="3" r="A267">
         <v>4118</v>
       </c>
       <c t="s" s="6" r="B267">
@@ -33980,7 +33980,7 @@
       </c>
     </row>
     <row r="268">
-      <c t="s" s="2" r="A268">
+      <c t="s" s="3" r="A268">
         <v>4121</v>
       </c>
       <c t="s" s="6" r="B268">
@@ -34058,7 +34058,7 @@
       </c>
     </row>
     <row r="269">
-      <c t="s" s="2" r="A269">
+      <c t="s" s="3" r="A269">
         <v>4125</v>
       </c>
       <c t="s" s="6" r="B269">
@@ -34136,7 +34136,7 @@
       </c>
     </row>
     <row r="270">
-      <c t="s" s="2" r="A270">
+      <c t="s" s="3" r="A270">
         <v>4128</v>
       </c>
       <c t="s" s="6" r="B270">
@@ -34214,7 +34214,7 @@
       </c>
     </row>
     <row r="271">
-      <c t="s" s="2" r="A271">
+      <c t="s" s="3" r="A271">
         <v>4131</v>
       </c>
       <c t="s" s="6" r="B271">
@@ -34292,7 +34292,7 @@
       </c>
     </row>
     <row r="272">
-      <c t="s" s="2" r="A272">
+      <c t="s" s="3" r="A272">
         <v>4153</v>
       </c>
       <c t="s" s="6" r="B272">
@@ -34370,7 +34370,7 @@
       </c>
     </row>
     <row r="273">
-      <c t="s" s="2" r="A273">
+      <c t="s" s="3" r="A273">
         <v>4177</v>
       </c>
       <c t="s" s="6" r="B273">
@@ -34450,7 +34450,7 @@
       </c>
     </row>
     <row r="274">
-      <c t="s" s="2" r="A274">
+      <c t="s" s="3" r="A274">
         <v>4185</v>
       </c>
       <c t="s" s="6" r="B274">
@@ -34530,7 +34530,7 @@
       </c>
     </row>
     <row r="275">
-      <c t="s" s="2" r="A275">
+      <c t="s" s="3" r="A275">
         <v>4191</v>
       </c>
       <c t="s" s="6" r="B275">
@@ -34608,7 +34608,7 @@
       </c>
     </row>
     <row r="276">
-      <c t="s" s="2" r="A276">
+      <c t="s" s="3" r="A276">
         <v>4213</v>
       </c>
       <c t="s" s="6" r="B276">
@@ -34686,7 +34686,7 @@
       </c>
     </row>
     <row r="277">
-      <c t="s" s="2" r="A277">
+      <c t="s" s="3" r="A277">
         <v>4238</v>
       </c>
       <c t="s" s="6" r="B277">
@@ -34764,7 +34764,7 @@
       </c>
     </row>
     <row r="278">
-      <c t="s" s="2" r="A278">
+      <c t="s" s="3" r="A278">
         <v>4260</v>
       </c>
       <c t="s" s="6" r="B278">
@@ -34842,7 +34842,7 @@
       </c>
     </row>
     <row r="279">
-      <c t="s" s="2" r="A279">
+      <c t="s" s="3" r="A279">
         <v>4284</v>
       </c>
       <c t="s" s="6" r="B279">
@@ -34920,7 +34920,7 @@
       </c>
     </row>
     <row r="280">
-      <c t="s" s="2" r="A280">
+      <c t="s" s="3" r="A280">
         <v>4308</v>
       </c>
       <c t="s" s="6" r="B280">
@@ -35000,7 +35000,7 @@
       </c>
     </row>
     <row r="281">
-      <c t="s" s="2" r="A281">
+      <c t="s" s="3" r="A281">
         <v>4334</v>
       </c>
       <c t="s" s="6" r="B281">
@@ -35078,7 +35078,7 @@
       </c>
     </row>
     <row r="282">
-      <c t="s" s="2" r="A282">
+      <c t="s" s="3" r="A282">
         <v>4342</v>
       </c>
       <c t="s" s="6" r="B282">
@@ -35158,7 +35158,7 @@
       </c>
     </row>
     <row r="283">
-      <c t="s" s="2" r="A283">
+      <c t="s" s="3" r="A283">
         <v>4368</v>
       </c>
       <c t="s" s="6" r="B283">
@@ -35236,7 +35236,7 @@
       </c>
     </row>
     <row r="284">
-      <c t="s" s="2" r="A284">
+      <c t="s" s="3" r="A284">
         <v>4387</v>
       </c>
       <c t="s" s="6" r="B284">
@@ -35316,7 +35316,7 @@
       </c>
     </row>
     <row r="285">
-      <c t="s" s="2" r="A285">
+      <c t="s" s="3" r="A285">
         <v>4411</v>
       </c>
       <c t="s" s="6" r="B285">
@@ -35392,7 +35392,7 @@
       </c>
     </row>
     <row r="286">
-      <c t="s" s="2" r="A286">
+      <c t="s" s="3" r="A286">
         <v>4427</v>
       </c>
       <c t="s" s="6" r="B286">
@@ -35472,7 +35472,7 @@
       </c>
     </row>
     <row r="287">
-      <c t="s" s="2" r="A287">
+      <c t="s" s="3" r="A287">
         <v>4443</v>
       </c>
       <c t="s" s="6" r="B287">
@@ -35552,7 +35552,7 @@
       </c>
     </row>
     <row r="288">
-      <c t="s" s="2" r="A288">
+      <c t="s" s="3" r="A288">
         <v>4450</v>
       </c>
       <c t="s" s="6" r="B288">
@@ -35626,7 +35626,7 @@
       </c>
     </row>
     <row r="289">
-      <c t="s" s="2" r="A289">
+      <c t="s" s="3" r="A289">
         <v>4472</v>
       </c>
       <c t="s" s="6" r="B289">
@@ -35706,7 +35706,7 @@
       </c>
     </row>
     <row r="290">
-      <c t="s" s="2" r="A290">
+      <c t="s" s="3" r="A290">
         <v>4494</v>
       </c>
       <c t="s" s="6" r="B290">
@@ -35782,7 +35782,7 @@
       </c>
     </row>
     <row r="291">
-      <c t="s" s="2" r="A291">
+      <c t="s" s="3" r="A291">
         <v>4514</v>
       </c>
       <c t="s" s="6" r="B291">
@@ -35862,7 +35862,7 @@
       </c>
     </row>
     <row r="292">
-      <c t="s" s="2" r="A292">
+      <c t="s" s="3" r="A292">
         <v>4525</v>
       </c>
       <c t="s" s="6" r="B292">
@@ -35940,7 +35940,7 @@
       </c>
     </row>
     <row r="293">
-      <c t="s" s="2" r="A293">
+      <c t="s" s="3" r="A293">
         <v>4548</v>
       </c>
       <c t="s" s="6" r="B293">
@@ -36020,7 +36020,7 @@
       </c>
     </row>
     <row r="294">
-      <c t="s" s="2" r="A294">
+      <c t="s" s="3" r="A294">
         <v>4565</v>
       </c>
       <c t="s" s="6" r="B294">
@@ -36098,7 +36098,7 @@
       </c>
     </row>
     <row r="295">
-      <c t="s" s="2" r="A295">
+      <c t="s" s="3" r="A295">
         <v>4590</v>
       </c>
       <c t="s" s="6" r="B295">
@@ -36176,7 +36176,7 @@
       </c>
     </row>
     <row r="296">
-      <c t="s" s="2" r="A296">
+      <c t="s" s="3" r="A296">
         <v>4615</v>
       </c>
       <c t="s" s="6" r="B296">
@@ -36254,7 +36254,7 @@
       </c>
     </row>
     <row r="297">
-      <c t="s" s="2" r="A297">
+      <c t="s" s="3" r="A297">
         <v>4637</v>
       </c>
       <c t="s" s="6" r="B297">
@@ -36332,7 +36332,7 @@
       </c>
     </row>
     <row r="298">
-      <c t="s" s="2" r="A298">
+      <c t="s" s="3" r="A298">
         <v>4662</v>
       </c>
       <c t="s" s="6" r="B298">
@@ -36410,7 +36410,7 @@
       </c>
     </row>
     <row r="299">
-      <c t="s" s="2" r="A299">
+      <c t="s" s="3" r="A299">
         <v>4685</v>
       </c>
       <c t="s" s="6" r="B299">
@@ -36488,7 +36488,7 @@
       </c>
     </row>
     <row r="300">
-      <c t="s" s="2" r="A300">
+      <c t="s" s="3" r="A300">
         <v>4710</v>
       </c>
       <c t="s" s="6" r="B300">
@@ -36566,7 +36566,7 @@
       </c>
     </row>
     <row r="301">
-      <c t="s" s="2" r="A301">
+      <c t="s" s="3" r="A301">
         <v>4723</v>
       </c>
       <c t="s" s="6" r="B301">
@@ -36644,7 +36644,7 @@
       </c>
     </row>
     <row r="302">
-      <c t="s" s="2" r="A302">
+      <c t="s" s="3" r="A302">
         <v>4747</v>
       </c>
       <c t="s" s="6" r="B302">
@@ -36722,7 +36722,7 @@
       </c>
     </row>
     <row r="303">
-      <c t="s" s="2" r="A303">
+      <c t="s" s="3" r="A303">
         <v>4772</v>
       </c>
       <c t="s" s="6" r="B303">
@@ -36800,7 +36800,7 @@
       </c>
     </row>
     <row r="304">
-      <c t="s" s="2" r="A304">
+      <c t="s" s="3" r="A304">
         <v>4796</v>
       </c>
       <c t="s" s="6" r="B304">
@@ -36878,7 +36878,7 @@
       </c>
     </row>
     <row r="305">
-      <c t="s" s="2" r="A305">
+      <c t="s" s="3" r="A305">
         <v>4821</v>
       </c>
       <c t="s" s="6" r="B305">
@@ -36956,7 +36956,7 @@
       </c>
     </row>
     <row r="306">
-      <c t="s" s="2" r="A306">
+      <c t="s" s="3" r="A306">
         <v>4845</v>
       </c>
       <c t="s" s="6" r="B306">
@@ -37034,7 +37034,7 @@
       </c>
     </row>
     <row r="307">
-      <c t="s" s="2" r="A307">
+      <c t="s" s="3" r="A307">
         <v>4869</v>
       </c>
       <c t="s" s="6" r="B307">
@@ -37112,7 +37112,7 @@
       </c>
     </row>
     <row r="308">
-      <c t="s" s="2" r="A308">
+      <c t="s" s="3" r="A308">
         <v>4893</v>
       </c>
       <c t="s" s="6" r="B308">
@@ -37190,7 +37190,7 @@
       </c>
     </row>
     <row r="309">
-      <c t="s" s="2" r="A309">
+      <c t="s" s="3" r="A309">
         <v>4918</v>
       </c>
       <c t="s" s="6" r="B309">
@@ -37268,7 +37268,7 @@
       </c>
     </row>
     <row r="310">
-      <c t="s" s="2" r="A310">
+      <c t="s" s="3" r="A310">
         <v>4943</v>
       </c>
       <c t="s" s="6" r="B310">
@@ -37348,7 +37348,7 @@
       </c>
     </row>
     <row r="311">
-      <c t="s" s="2" r="A311">
+      <c t="s" s="3" r="A311">
         <v>4961</v>
       </c>
       <c t="s" s="6" r="B311">
@@ -37426,7 +37426,7 @@
       </c>
     </row>
     <row r="312">
-      <c t="s" s="2" r="A312">
+      <c t="s" s="3" r="A312">
         <v>4975</v>
       </c>
       <c t="s" s="6" r="B312">
@@ -37504,7 +37504,7 @@
       </c>
     </row>
     <row r="313">
-      <c t="s" s="2" r="A313">
+      <c t="s" s="3" r="A313">
         <v>4979</v>
       </c>
       <c t="s" s="6" r="B313">
@@ -37582,7 +37582,7 @@
       </c>
     </row>
     <row r="314">
-      <c t="s" s="2" r="A314">
+      <c t="s" s="3" r="A314">
         <v>4985</v>
       </c>
       <c t="s" s="6" r="B314">
@@ -37660,7 +37660,7 @@
       </c>
     </row>
     <row r="315">
-      <c t="s" s="2" r="A315">
+      <c t="s" s="3" r="A315">
         <v>4999</v>
       </c>
       <c t="s" s="6" r="B315">
@@ -37738,7 +37738,7 @@
       </c>
     </row>
     <row r="316">
-      <c t="s" s="2" r="A316">
+      <c t="s" s="3" r="A316">
         <v>5010</v>
       </c>
       <c t="s" s="6" r="B316">
@@ -37816,7 +37816,7 @@
       </c>
     </row>
     <row r="317">
-      <c t="s" s="2" r="A317">
+      <c t="s" s="3" r="A317">
         <v>5028</v>
       </c>
       <c t="s" s="6" r="B317">
@@ -37894,7 +37894,7 @@
       </c>
     </row>
     <row r="318">
-      <c t="s" s="2" r="A318">
+      <c t="s" s="3" r="A318">
         <v>5046</v>
       </c>
       <c t="s" s="6" r="B318">
@@ -37974,7 +37974,7 @@
       </c>
     </row>
     <row customHeight="1" r="319" ht="26.25">
-      <c t="s" s="2" r="A319">
+      <c t="s" s="3" r="A319">
         <v>5069</v>
       </c>
       <c t="s" s="6" r="B319">
@@ -38052,7 +38052,7 @@
       </c>
     </row>
     <row customHeight="1" r="320" ht="26.25">
-      <c t="s" s="2" r="A320">
+      <c t="s" s="3" r="A320">
         <v>5094</v>
       </c>
       <c t="s" s="6" r="B320">
@@ -38130,7 +38130,7 @@
       </c>
     </row>
     <row customHeight="1" r="321" ht="26.25">
-      <c t="s" s="2" r="A321">
+      <c t="s" s="3" r="A321">
         <v>5117</v>
       </c>
       <c t="s" s="6" r="B321">
@@ -38208,7 +38208,7 @@
       </c>
     </row>
     <row customHeight="1" r="322" ht="26.25">
-      <c t="s" s="2" r="A322">
+      <c t="s" s="3" r="A322">
         <v>5142</v>
       </c>
       <c t="s" s="6" r="B322">
@@ -38286,7 +38286,7 @@
       </c>
     </row>
     <row r="323">
-      <c s="2" r="A323"/>
+      <c s="3" r="A323"/>
       <c s="6" r="B323"/>
       <c s="6" r="C323"/>
       <c s="6" r="D323"/>
@@ -38314,7 +38314,7 @@
       <c s="6" r="Z323"/>
     </row>
     <row r="324">
-      <c s="2" r="A324"/>
+      <c s="3" r="A324"/>
       <c s="6" r="B324"/>
       <c s="6" r="C324"/>
       <c s="6" r="D324"/>
@@ -38372,7 +38372,7 @@
       <c t="s" s="8" r="A1">
         <v>3889</v>
       </c>
-      <c t="s" s="4" r="B1">
+      <c t="s" s="5" r="B1">
         <v>5167</v>
       </c>
       <c s="8" r="C1"/>
@@ -38399,11 +38399,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>English</v>
       </c>
-      <c s="1" r="B2">
+      <c s="2" r="B2">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>1</v>
       </c>
-      <c t="str" s="3" r="C2">
+      <c t="str" s="4" r="C2">
         <f>REPT("█", INT((B2*15)))</f>
         <v>███████████████</v>
       </c>
@@ -38413,11 +38413,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Turkish</v>
       </c>
-      <c s="1" r="B3">
+      <c s="2" r="B3">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.96875</v>
       </c>
-      <c t="str" s="3" r="C3">
+      <c t="str" s="4" r="C3">
         <f>REPT("█", INT((B3*15)))</f>
         <v>██████████████</v>
       </c>
@@ -38427,11 +38427,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Vietnamese</v>
       </c>
-      <c s="1" r="B4">
+      <c s="2" r="B4">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.971875</v>
       </c>
-      <c t="str" s="3" r="C4">
+      <c t="str" s="4" r="C4">
         <f>REPT("█", INT((B4*15)))</f>
         <v>██████████████</v>
       </c>
@@ -38441,11 +38441,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Japanese</v>
       </c>
-      <c s="1" r="B5">
+      <c s="2" r="B5">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.90625</v>
       </c>
-      <c t="str" s="3" r="C5">
+      <c t="str" s="4" r="C5">
         <f>REPT("█", INT((B5*15)))</f>
         <v>█████████████</v>
       </c>
@@ -38455,11 +38455,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Polish</v>
       </c>
-      <c s="1" r="B6">
+      <c s="2" r="B6">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>1</v>
       </c>
-      <c t="str" s="3" r="C6">
+      <c t="str" s="4" r="C6">
         <f>REPT("█", INT((B6*15)))</f>
         <v>███████████████</v>
       </c>
@@ -38469,11 +38469,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Romanian</v>
       </c>
-      <c s="1" r="B7">
+      <c s="2" r="B7">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.471875</v>
       </c>
-      <c t="str" s="3" r="C7">
+      <c t="str" s="4" r="C7">
         <f>REPT("█", INT((B7*15)))</f>
         <v>███████</v>
       </c>
@@ -38483,11 +38483,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Danish</v>
       </c>
-      <c s="1" r="B8">
+      <c s="2" r="B8">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.971875</v>
       </c>
-      <c t="str" s="3" r="C8">
+      <c t="str" s="4" r="C8">
         <f>REPT("█", INT((B8*15)))</f>
         <v>██████████████</v>
       </c>
@@ -38497,11 +38497,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Arabic (Bahrain)</v>
       </c>
-      <c s="1" r="B9">
+      <c s="2" r="B9">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.359375</v>
       </c>
-      <c t="str" s="3" r="C9">
+      <c t="str" s="4" r="C9">
         <f>REPT("█", INT((B9*15)))</f>
         <v>█████</v>
       </c>
@@ -38511,11 +38511,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Italian</v>
       </c>
-      <c s="1" r="B10">
+      <c s="2" r="B10">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.83125</v>
       </c>
-      <c t="str" s="3" r="C10">
+      <c t="str" s="4" r="C10">
         <f>REPT("█", INT((B10*15)))</f>
         <v>████████████</v>
       </c>
@@ -38525,11 +38525,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Hebrew</v>
       </c>
-      <c s="1" r="B11">
+      <c s="2" r="B11">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.690625</v>
       </c>
-      <c t="str" s="3" r="C11">
+      <c t="str" s="4" r="C11">
         <f>REPT("█", INT((B11*15)))</f>
         <v>██████████</v>
       </c>
@@ -38539,11 +38539,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Spanish</v>
       </c>
-      <c s="1" r="B12">
+      <c s="2" r="B12">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.925</v>
       </c>
-      <c t="str" s="3" r="C12">
+      <c t="str" s="4" r="C12">
         <f>REPT("█", INT((B12*15)))</f>
         <v>█████████████</v>
       </c>
@@ -38553,11 +38553,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>French</v>
       </c>
-      <c s="1" r="B13">
+      <c s="2" r="B13">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.996875</v>
       </c>
-      <c t="str" s="3" r="C13">
+      <c t="str" s="4" r="C13">
         <f>REPT("█", INT((B13*15)))</f>
         <v>██████████████</v>
       </c>
@@ -38567,11 +38567,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Russian</v>
       </c>
-      <c s="1" r="B14">
+      <c s="2" r="B14">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.978125</v>
       </c>
-      <c t="str" s="3" r="C14">
+      <c t="str" s="4" r="C14">
         <f>REPT("█", INT((B14*15)))</f>
         <v>██████████████</v>
       </c>
@@ -38581,11 +38581,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>German</v>
       </c>
-      <c s="1" r="B15">
+      <c s="2" r="B15">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.61875</v>
       </c>
-      <c t="str" s="3" r="C15">
+      <c t="str" s="4" r="C15">
         <f>REPT("█", INT((B15*15)))</f>
         <v>█████████</v>
       </c>
@@ -38595,11 +38595,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Dutch</v>
       </c>
-      <c s="1" r="B16">
+      <c s="2" r="B16">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.13125</v>
       </c>
-      <c t="str" s="3" r="C16">
+      <c t="str" s="4" r="C16">
         <f>REPT("█", INT((B16*15)))</f>
         <v>█</v>
       </c>
@@ -38609,11 +38609,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Hungarian</v>
       </c>
-      <c s="1" r="B17">
+      <c s="2" r="B17">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>1</v>
       </c>
-      <c t="str" s="3" r="C17">
+      <c t="str" s="4" r="C17">
         <f>REPT("█", INT((B17*15)))</f>
         <v>███████████████</v>
       </c>
@@ -38623,11 +38623,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Portuguese (Brazil)</v>
       </c>
-      <c s="1" r="B18">
+      <c s="2" r="B18">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.734375</v>
       </c>
-      <c t="str" s="3" r="C18">
+      <c t="str" s="4" r="C18">
         <f>REPT("█", INT((B18*15)))</f>
         <v>███████████</v>
       </c>
@@ -38637,11 +38637,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Chinese (S)</v>
       </c>
-      <c s="1" r="B19">
+      <c s="2" r="B19">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.68125</v>
       </c>
-      <c t="str" s="3" r="C19">
+      <c t="str" s="4" r="C19">
         <f>REPT("█", INT((B19*15)))</f>
         <v>██████████</v>
       </c>
@@ -38651,11 +38651,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Slovak</v>
       </c>
-      <c s="1" r="B20">
+      <c s="2" r="B20">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>1</v>
       </c>
-      <c t="str" s="3" r="C20">
+      <c t="str" s="4" r="C20">
         <f>REPT("█", INT((B20*15)))</f>
         <v>███████████████</v>
       </c>
@@ -38665,11 +38665,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Traditional Chinese</v>
       </c>
-      <c s="1" r="B21">
+      <c s="2" r="B21">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.859375</v>
       </c>
-      <c t="str" s="3" r="C21">
+      <c t="str" s="4" r="C21">
         <f>REPT("█", INT((B21*15)))</f>
         <v>████████████</v>
       </c>
@@ -38679,11 +38679,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Ukrainian</v>
       </c>
-      <c s="1" r="B22">
+      <c s="2" r="B22">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.575</v>
       </c>
-      <c t="str" s="3" r="C22">
+      <c t="str" s="4" r="C22">
         <f>REPT("█", INT((B22*15)))</f>
         <v>████████</v>
       </c>
@@ -38693,11 +38693,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Portuguese</v>
       </c>
-      <c s="1" r="B23">
+      <c s="2" r="B23">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.684375</v>
       </c>
-      <c t="str" s="3" r="C23">
+      <c t="str" s="4" r="C23">
         <f>REPT("█", INT((B23*15)))</f>
         <v>██████████</v>
       </c>
@@ -38707,11 +38707,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Swedish</v>
       </c>
-      <c s="1" r="B24">
+      <c s="2" r="B24">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.684375</v>
       </c>
-      <c t="str" s="3" r="C24">
+      <c t="str" s="4" r="C24">
         <f>REPT("█", INT((B24*15)))</f>
         <v>██████████</v>
       </c>
@@ -38721,11 +38721,11 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Persian</v>
       </c>
-      <c s="1" r="B25">
+      <c s="2" r="B25">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.69375</v>
       </c>
-      <c t="str" s="3" r="C25">
+      <c t="str" s="4" r="C25">
         <f>REPT("█", INT((B25*15)))</f>
         <v>██████████</v>
       </c>
@@ -38735,236 +38735,236 @@
         <f>INDIRECT(CONCAT("Sheet1!R1C", ROW()))</f>
         <v>Catalan</v>
       </c>
-      <c s="1" r="B26">
+      <c s="2" r="B26">
         <f>1.0 -( COUNTBLANK(INDIRECT(CONCATENATE("Sheet1!R3C", ROW(), ":R", COUNTA(Sheet1!$A$3:$A$1006), "C", ROW()))) / COUNTA(Sheet1!$A$3:$A$1006))</f>
         <v>0.98125</v>
       </c>
-      <c t="str" s="3" r="C26">
+      <c t="str" s="4" r="C26">
         <f>REPT("█", INT((B26*15)))</f>
         <v>██████████████</v>
       </c>
     </row>
     <row r="27">
-      <c s="1" r="B27"/>
+      <c s="2" r="B27"/>
     </row>
     <row r="28">
-      <c s="1" r="B28"/>
+      <c s="2" r="B28"/>
     </row>
     <row r="29">
-      <c s="1" r="B29"/>
+      <c s="2" r="B29"/>
     </row>
     <row r="30">
-      <c s="1" r="B30"/>
+      <c s="2" r="B30"/>
     </row>
     <row r="31">
-      <c s="1" r="B31"/>
+      <c s="2" r="B31"/>
     </row>
     <row r="32">
-      <c s="1" r="B32"/>
+      <c s="2" r="B32"/>
     </row>
     <row r="33">
-      <c s="1" r="B33"/>
+      <c s="2" r="B33"/>
     </row>
     <row r="34">
-      <c s="1" r="B34"/>
+      <c s="2" r="B34"/>
     </row>
     <row r="35">
-      <c s="1" r="B35"/>
+      <c s="2" r="B35"/>
     </row>
     <row r="36">
-      <c s="1" r="B36"/>
+      <c s="2" r="B36"/>
     </row>
     <row r="37">
-      <c s="1" r="B37"/>
+      <c s="2" r="B37"/>
     </row>
     <row r="38">
-      <c s="1" r="B38"/>
+      <c s="2" r="B38"/>
     </row>
     <row r="39">
-      <c s="1" r="B39"/>
+      <c s="2" r="B39"/>
     </row>
     <row r="40">
-      <c s="1" r="B40"/>
+      <c s="2" r="B40"/>
     </row>
     <row r="41">
-      <c s="1" r="B41"/>
+      <c s="2" r="B41"/>
     </row>
     <row r="42">
-      <c s="1" r="B42"/>
+      <c s="2" r="B42"/>
     </row>
     <row r="43">
-      <c s="1" r="B43"/>
+      <c s="2" r="B43"/>
     </row>
     <row r="44">
-      <c s="1" r="B44"/>
+      <c s="2" r="B44"/>
     </row>
     <row r="45">
-      <c s="1" r="B45"/>
+      <c s="2" r="B45"/>
     </row>
     <row r="46">
-      <c s="1" r="B46"/>
+      <c s="2" r="B46"/>
     </row>
     <row r="47">
-      <c s="1" r="B47"/>
+      <c s="2" r="B47"/>
     </row>
     <row r="48">
-      <c s="1" r="B48"/>
+      <c s="2" r="B48"/>
     </row>
     <row r="49">
-      <c s="1" r="B49"/>
+      <c s="2" r="B49"/>
     </row>
     <row r="50">
-      <c s="1" r="B50"/>
+      <c s="2" r="B50"/>
     </row>
     <row r="51">
-      <c s="1" r="B51"/>
+      <c s="2" r="B51"/>
     </row>
     <row r="52">
-      <c s="1" r="B52"/>
+      <c s="2" r="B52"/>
     </row>
     <row r="53">
-      <c s="1" r="B53"/>
+      <c s="2" r="B53"/>
     </row>
     <row r="54">
-      <c s="1" r="B54"/>
+      <c s="2" r="B54"/>
     </row>
     <row r="55">
-      <c s="1" r="B55"/>
+      <c s="2" r="B55"/>
     </row>
     <row r="56">
-      <c s="1" r="B56"/>
+      <c s="2" r="B56"/>
     </row>
     <row r="57">
-      <c s="1" r="B57"/>
+      <c s="2" r="B57"/>
     </row>
     <row r="58">
-      <c s="1" r="B58"/>
+      <c s="2" r="B58"/>
     </row>
     <row r="59">
-      <c s="1" r="B59"/>
+      <c s="2" r="B59"/>
     </row>
     <row r="60">
-      <c s="1" r="B60"/>
+      <c s="2" r="B60"/>
     </row>
     <row r="61">
-      <c s="1" r="B61"/>
+      <c s="2" r="B61"/>
     </row>
     <row r="62">
-      <c s="1" r="B62"/>
+      <c s="2" r="B62"/>
     </row>
     <row r="63">
-      <c s="1" r="B63"/>
+      <c s="2" r="B63"/>
     </row>
     <row r="64">
-      <c s="1" r="B64"/>
+      <c s="2" r="B64"/>
     </row>
     <row r="65">
-      <c s="1" r="B65"/>
+      <c s="2" r="B65"/>
     </row>
     <row r="66">
-      <c s="1" r="B66"/>
+      <c s="2" r="B66"/>
     </row>
     <row r="67">
-      <c s="1" r="B67"/>
+      <c s="2" r="B67"/>
     </row>
     <row r="68">
-      <c s="1" r="B68"/>
+      <c s="2" r="B68"/>
     </row>
     <row r="69">
-      <c s="1" r="B69"/>
+      <c s="2" r="B69"/>
     </row>
     <row r="70">
-      <c s="1" r="B70"/>
+      <c s="2" r="B70"/>
     </row>
     <row r="71">
-      <c s="1" r="B71"/>
+      <c s="2" r="B71"/>
     </row>
     <row r="72">
-      <c s="1" r="B72"/>
+      <c s="2" r="B72"/>
     </row>
     <row r="73">
-      <c s="1" r="B73"/>
+      <c s="2" r="B73"/>
     </row>
     <row r="74">
-      <c s="1" r="B74"/>
+      <c s="2" r="B74"/>
     </row>
     <row r="75">
-      <c s="1" r="B75"/>
+      <c s="2" r="B75"/>
     </row>
     <row r="76">
-      <c s="1" r="B76"/>
+      <c s="2" r="B76"/>
     </row>
     <row r="77">
-      <c s="1" r="B77"/>
+      <c s="2" r="B77"/>
     </row>
     <row r="78">
-      <c s="1" r="B78"/>
+      <c s="2" r="B78"/>
     </row>
     <row r="79">
-      <c s="1" r="B79"/>
+      <c s="2" r="B79"/>
     </row>
     <row r="80">
-      <c s="1" r="B80"/>
+      <c s="2" r="B80"/>
     </row>
     <row r="81">
-      <c s="1" r="B81"/>
+      <c s="2" r="B81"/>
     </row>
     <row r="82">
-      <c s="1" r="B82"/>
+      <c s="2" r="B82"/>
     </row>
     <row r="83">
-      <c s="1" r="B83"/>
+      <c s="2" r="B83"/>
     </row>
     <row r="84">
-      <c s="1" r="B84"/>
+      <c s="2" r="B84"/>
     </row>
     <row r="85">
-      <c s="1" r="B85"/>
+      <c s="2" r="B85"/>
     </row>
     <row r="86">
-      <c s="1" r="B86"/>
+      <c s="2" r="B86"/>
     </row>
     <row r="87">
-      <c s="1" r="B87"/>
+      <c s="2" r="B87"/>
     </row>
     <row r="88">
-      <c s="1" r="B88"/>
+      <c s="2" r="B88"/>
     </row>
     <row r="89">
-      <c s="1" r="B89"/>
+      <c s="2" r="B89"/>
     </row>
     <row r="90">
-      <c s="1" r="B90"/>
+      <c s="2" r="B90"/>
     </row>
     <row r="91">
-      <c s="1" r="B91"/>
+      <c s="2" r="B91"/>
     </row>
     <row r="92">
-      <c s="1" r="B92"/>
+      <c s="2" r="B92"/>
     </row>
     <row r="93">
-      <c s="1" r="B93"/>
+      <c s="2" r="B93"/>
     </row>
     <row r="94">
-      <c s="1" r="B94"/>
+      <c s="2" r="B94"/>
     </row>
     <row r="95">
-      <c s="1" r="B95"/>
+      <c s="2" r="B95"/>
     </row>
     <row r="96">
-      <c s="1" r="B96"/>
+      <c s="2" r="B96"/>
     </row>
     <row r="97">
-      <c s="1" r="B97"/>
+      <c s="2" r="B97"/>
     </row>
     <row r="98">
-      <c s="1" r="B98"/>
+      <c s="2" r="B98"/>
     </row>
     <row r="99">
-      <c s="1" r="B99"/>
+      <c s="2" r="B99"/>
     </row>
     <row r="100">
-      <c s="1" r="B100"/>
+      <c s="2" r="B100"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>